<commit_message>
T4B - Com todas as tabelas
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3953D645-38BD-4FFA-AD86-F879CD2AE914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B90DECF-384B-46FF-9C09-124F9A9B4523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Carga</t>
   </si>
@@ -72,6 +72,33 @@
   <si>
     <t>diametro (φ) (m)</t>
   </si>
+  <si>
+    <t>Média</t>
+  </si>
+  <si>
+    <t>Desvio padrão</t>
+  </si>
+  <si>
+    <t>u(média)</t>
+  </si>
+  <si>
+    <t>D (m)</t>
+  </si>
+  <si>
+    <t>u(D) (m)</t>
+  </si>
+  <si>
+    <t>L0 (m)</t>
+  </si>
+  <si>
+    <t>u(L0) (m)</t>
+  </si>
+  <si>
+    <t>u(h) (m)</t>
+  </si>
+  <si>
+    <t>h (m)</t>
+  </si>
 </sst>
 </file>
 
@@ -86,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -99,14 +126,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -129,18 +150,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2300,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83617AA6-E6F3-42B7-BA6C-E56FF542CF9F}">
-  <dimension ref="B2:O45"/>
+  <dimension ref="B2:P50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2311,7 +2396,9 @@
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
     <col min="11" max="12" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
@@ -2322,155 +2409,163 @@
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="H9" s="11"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
@@ -2480,110 +2575,394 @@
       <c r="D30" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="1" t="s">
+      <c r="F30" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
+      <c r="H30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J30" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L30" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P30" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="3" t="e">
+        <f>AVERAGE(F31:F39)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I31" s="3" t="e">
+        <f>_xlfn.STDEV.P(F31:F39)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J31" s="3" t="e">
+        <f>I31/SQRT(COUNT(F31:F39))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="3" t="e">
+        <f>AVERAGE(L31:L39)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O31" s="3" t="e">
+        <f>_xlfn.STDEV.P(L31:L39)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P31" s="3" t="e">
+        <f>O31/SQRT(COUNT(L31:L39))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+    </row>
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="4"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
+    </row>
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="F41" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="N41" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P41" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="3" t="e">
+        <f>AVERAGE(F42:F50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I42" s="3" t="e">
+        <f>_xlfn.STDEV.P(F42:F50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J42" s="3" t="e">
+        <f>I42/SQRT(COUNT(F42:F50))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="3" t="e">
+        <f>AVERAGE(L42:L50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="O42" s="3" t="e">
+        <f>_xlfn.STDEV.P(L42:L50)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P42" s="3" t="e">
+        <f>O42/SQRT(COUNT(L42:L50))</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="4"/>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+    </row>
+    <row r="49" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="4"/>
+      <c r="O49" s="4"/>
+      <c r="P49" s="4"/>
+    </row>
+    <row r="50" spans="6:16" x14ac:dyDescent="0.3">
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+      <c r="P50" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="14">
+    <mergeCell ref="P31:P39"/>
+    <mergeCell ref="N42:N50"/>
+    <mergeCell ref="O42:O50"/>
+    <mergeCell ref="P42:P50"/>
+    <mergeCell ref="H42:H50"/>
+    <mergeCell ref="I42:I50"/>
+    <mergeCell ref="J42:J50"/>
+    <mergeCell ref="N31:N39"/>
+    <mergeCell ref="O31:O39"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="K2:O2"/>
+    <mergeCell ref="H31:H39"/>
+    <mergeCell ref="I31:I39"/>
+    <mergeCell ref="J31:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Completamento dos dados (1)
-Colocação dos valores na tabela.
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive - Universidade do Porto\Ambiente de Trabalho\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE0C6194-2F2B-4372-9A93-11544CA86D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA11C410-C8BE-4E6F-A36F-E778F0AFF54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>Carga</t>
   </si>
@@ -70,9 +70,6 @@
     <t>u(φ) (m)</t>
   </si>
   <si>
-    <t>diametro (φ) (m)</t>
-  </si>
-  <si>
     <t>Média</t>
   </si>
   <si>
@@ -86,18 +83,6 @@
   </si>
   <si>
     <t>u(D) (m)</t>
-  </si>
-  <si>
-    <t>L0 (m)</t>
-  </si>
-  <si>
-    <t>u(L0) (m)</t>
-  </si>
-  <si>
-    <t>u(h) (m)</t>
-  </si>
-  <si>
-    <t>h (m)</t>
   </si>
   <si>
     <t>1+2</t>
@@ -129,14 +114,45 @@
   <si>
     <t>L0</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>diametro (φ) (cm)</t>
+  </si>
+  <si>
+    <t>h (cm)</t>
+  </si>
+  <si>
+    <t>u(h) (cm)</t>
+  </si>
+  <si>
+    <t>L0 (cm)</t>
+  </si>
+  <si>
+    <t>u(L0) (cm)</t>
+  </si>
+  <si>
+    <t>0,15*</t>
+  </si>
+  <si>
+    <t>* Incerteza obtida por cálculo, devido a oscilações no valor apresentado no instrumento de medida.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -184,43 +200,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -230,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -250,14 +229,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -265,8 +244,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -401,20 +386,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$F$4:$F$12</c:f>
@@ -797,20 +768,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$O$4:$O$12</c:f>
@@ -2563,23 +2520,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83617AA6-E6F3-42B7-BA6C-E56FF542CF9F}">
-  <dimension ref="B2:P50"/>
+  <dimension ref="B2:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
-    <col min="11" max="12" width="12.5546875" customWidth="1"/>
-    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="10" t="s">
         <v>0</v>
       </c>
@@ -2595,7 +2554,7 @@
       <c r="N2" s="11"/>
       <c r="O2" s="11"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2611,8 +2570,8 @@
       <c r="F3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="12" t="s">
-        <v>30</v>
+      <c r="H3" s="9" t="s">
+        <v>25</v>
       </c>
       <c r="I3">
         <v>38.5</v>
@@ -2632,8 +2591,12 @@
       <c r="O3" s="4" t="s">
         <v>5</v>
       </c>
+      <c r="Q3" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -2643,13 +2606,15 @@
       <c r="D4" s="2">
         <v>38.299999999999997</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F4" s="2">
         <f>$I$3-D4</f>
         <v>0.20000000000000284</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L4" s="2">
         <v>9997.4</v>
@@ -2657,15 +2622,19 @@
       <c r="M4" s="2">
         <v>33</v>
       </c>
-      <c r="N4" s="2"/>
+      <c r="N4" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O4" s="2">
         <f>M4-$I$3</f>
         <v>-5.5</v>
       </c>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C5" s="2">
         <v>3003.4</v>
@@ -2673,16 +2642,15 @@
       <c r="D5" s="2">
         <v>37.700000000000003</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F5" s="2">
         <f t="shared" ref="F5:F12" si="0">$I$3-D5</f>
         <v>0.79999999999999716</v>
       </c>
-      <c r="I5">
-        <v>6</v>
-      </c>
       <c r="K5" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="L5" s="2">
         <v>8996.7000000000007</v>
@@ -2690,15 +2658,19 @@
       <c r="M5" s="2">
         <v>33.5</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O5" s="2">
         <f t="shared" ref="O5:O12" si="1">M5-$I$3</f>
         <v>-5</v>
       </c>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C6" s="2">
         <v>4000.4</v>
@@ -2706,13 +2678,15 @@
       <c r="D6" s="2">
         <v>37</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="L6" s="2">
         <v>7999.15</v>
@@ -2720,15 +2694,19 @@
       <c r="M6" s="2">
         <v>34</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O6" s="2">
         <f t="shared" si="1"/>
         <v>-4.5</v>
       </c>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2">
         <v>5002.1000000000004</v>
@@ -2736,13 +2714,15 @@
       <c r="D7" s="2">
         <v>36.799999999999997</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
         <v>1.7000000000000028</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="L7" s="2">
         <v>6999.6</v>
@@ -2750,15 +2730,17 @@
       <c r="M7" s="2">
         <v>34.4</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O7" s="2">
         <f t="shared" si="1"/>
         <v>-4.1000000000000014</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C8" s="2">
         <v>6003.3</v>
@@ -2766,13 +2748,15 @@
       <c r="D8" s="2">
         <v>36.299999999999997</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
         <v>2.2000000000000028</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L8" s="2">
         <v>6003.3</v>
@@ -2780,15 +2764,17 @@
       <c r="M8" s="2">
         <v>34.799999999999997</v>
       </c>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O8" s="2">
         <f t="shared" si="1"/>
         <v>-3.7000000000000028</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2">
         <v>6999.6</v>
@@ -2796,14 +2782,16 @@
       <c r="D9" s="2">
         <v>35.9</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
         <v>2.6000000000000014</v>
       </c>
       <c r="H9" s="6"/>
       <c r="K9" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L9" s="2">
         <v>5002.1000000000004</v>
@@ -2811,15 +2799,17 @@
       <c r="M9" s="2">
         <v>35.200000000000003</v>
       </c>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O9" s="2">
         <f t="shared" si="1"/>
         <v>-3.2999999999999972</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C10" s="2">
         <v>7999.15</v>
@@ -2827,13 +2817,15 @@
       <c r="D10" s="2">
         <v>34.4</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>4.1000000000000014</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="L10" s="2">
         <v>4000.4</v>
@@ -2841,15 +2833,17 @@
       <c r="M10" s="2">
         <v>36.200000000000003</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O10" s="2">
         <f t="shared" si="1"/>
         <v>-2.2999999999999972</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2">
         <v>8996.7000000000007</v>
@@ -2857,13 +2851,15 @@
       <c r="D11" s="2">
         <v>34</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
         <v>4.5</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="L11" s="2">
         <v>3003.4</v>
@@ -2871,15 +2867,17 @@
       <c r="M11" s="2">
         <v>37.1</v>
       </c>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O11" s="2">
         <f t="shared" si="1"/>
         <v>-1.3999999999999986</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12" s="2">
         <v>9997.4</v>
@@ -2887,7 +2885,9 @@
       <c r="D12" s="2">
         <v>33</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2">
+        <v>0.1</v>
+      </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
         <v>5.5</v>
@@ -2901,13 +2901,15 @@
       <c r="M12" s="2">
         <v>37.700000000000003</v>
       </c>
-      <c r="N12" s="2"/>
+      <c r="N12" s="2">
+        <v>0.1</v>
+      </c>
       <c r="O12" s="2">
         <f t="shared" si="1"/>
         <v>-0.79999999999999716</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3">
@@ -2916,460 +2918,394 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H30" s="4" t="s">
+      <c r="I30" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="4" t="s">
+      <c r="J30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J30" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M30" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N30" s="4" t="s">
+      <c r="L30" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="N30" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O30" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="O30" s="4" t="s">
+      <c r="P30" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="P30" s="4" t="s">
-        <v>14</v>
-      </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>1</v>
       </c>
       <c r="C31" s="2">
         <v>2005.75</v>
       </c>
-      <c r="D31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="7" t="e">
-        <f>AVERAGE(F31:F39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I31" s="7" t="e">
-        <f>_xlfn.STDEV.P(F31:F39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J31" s="7" t="e">
-        <f>I31/SQRT(COUNT(F31:F39))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="7" t="e">
-        <f>AVERAGE(L31:L39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O31" s="7" t="e">
-        <f>_xlfn.STDEV.P(L31:L39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P31" s="7" t="e">
-        <f>O31/SQRT(COUNT(L31:L39))</f>
-        <v>#DIV/0!</v>
+      <c r="D31" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F31" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H31" s="12">
+        <f>AVERAGE(F31:F36)</f>
+        <v>0.13025</v>
+      </c>
+      <c r="I31" s="12">
+        <f>_xlfn.STDEV.P(F31:F36)</f>
+        <v>1.4790199457749053E-3</v>
+      </c>
+      <c r="J31" s="12">
+        <f>I31/SQRT(COUNT(F31:F36))</f>
+        <v>7.3950997288745263E-4</v>
+      </c>
+      <c r="L31" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N31" s="12">
+        <f>AVERAGE(L31:L33)</f>
+        <v>38.533333333333331</v>
+      </c>
+      <c r="O31" s="12">
+        <f>_xlfn.STDEV.P(L31:L33)</f>
+        <v>4.7140452079103841E-2</v>
+      </c>
+      <c r="P31" s="12">
+        <f>O31/SQRT(COUNT(L31:L33))</f>
+        <v>2.7216552697591257E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>2</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="8"/>
-      <c r="O32" s="8"/>
-      <c r="P32" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="2">
+        <v>0.128</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="L32" s="2">
+        <v>38.6</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <v>3</v>
       </c>
       <c r="C33" s="2">
         <v>997</v>
       </c>
-      <c r="D33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="8"/>
-      <c r="P33" s="8"/>
+      <c r="D33" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="L33" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="2">
         <v>4</v>
       </c>
       <c r="C34" s="2">
         <v>1001.7</v>
       </c>
-      <c r="D34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="8"/>
-      <c r="P34" s="8"/>
+      <c r="D34" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F34" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="2">
         <v>5</v>
       </c>
       <c r="C35" s="2">
         <v>1001.2</v>
       </c>
-      <c r="D35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
+      <c r="D35" s="2">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <v>6</v>
       </c>
       <c r="C36" s="2">
         <v>996.3</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="8"/>
-      <c r="P36" s="8"/>
+      <c r="D36" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="L36" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="O36" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P36" s="8" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <v>7</v>
       </c>
       <c r="C37" s="2">
         <v>999.55</v>
       </c>
-      <c r="D37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
+      <c r="D37" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J37" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L37" s="2">
+        <v>22</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N37" s="12">
+        <f>AVERAGE(L37:L50)</f>
+        <v>22</v>
+      </c>
+      <c r="O37" s="12">
+        <f>_xlfn.STDEV.P(L37:L50)</f>
+        <v>0</v>
+      </c>
+      <c r="P37" s="12">
+        <f>O37/SQRT(COUNT(L37:L50))</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <v>8</v>
       </c>
       <c r="C38" s="2">
         <v>997.55</v>
       </c>
-      <c r="D38" s="2"/>
-      <c r="F38" s="2"/>
+      <c r="D38" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F38" s="2">
+        <v>252.1</v>
+      </c>
       <c r="G38" s="2"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="8"/>
-      <c r="P38" s="8"/>
+      <c r="H38" s="12">
+        <f>AVERAGE(F38:F50)</f>
+        <v>251.26666666666665</v>
+      </c>
+      <c r="I38" s="12">
+        <f>_xlfn.STDEV.P(F38:F50)</f>
+        <v>0.69442222186665081</v>
+      </c>
+      <c r="J38" s="12">
+        <f>I38/SQRT(COUNT(F38:F50))</f>
+        <v>0.40092485672596889</v>
+      </c>
+      <c r="L38" s="2">
+        <v>22</v>
+      </c>
+      <c r="M38" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N38" s="12"/>
+      <c r="O38" s="12"/>
+      <c r="P38" s="12"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <v>9</v>
       </c>
       <c r="C39" s="2">
         <v>1000.7</v>
       </c>
-      <c r="D39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="D39" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F39" s="2">
+        <v>250.4</v>
+      </c>
       <c r="G39" s="2"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="9"/>
-      <c r="O39" s="9"/>
-      <c r="P39" s="9"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="L39" s="2">
+        <v>22</v>
+      </c>
+      <c r="M39" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <v>10</v>
       </c>
       <c r="C40" s="2">
         <v>2003.35</v>
       </c>
-      <c r="D40" s="2"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
+      <c r="D40" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F40" s="2">
+        <v>251.3</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12"/>
+      <c r="J40" s="12"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="2">
         <v>11</v>
       </c>
       <c r="C41" s="2">
         <v>1999.1</v>
       </c>
-      <c r="D41" s="2"/>
-      <c r="F41" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="M41" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O41" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="P41" s="4" t="s">
-        <v>14</v>
+      <c r="D41" s="2">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="2">
         <v>12</v>
       </c>
       <c r="C42" s="2">
         <v>995.9</v>
       </c>
-      <c r="D42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="7" t="e">
-        <f>AVERAGE(F42:F50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I42" s="7" t="e">
-        <f>_xlfn.STDEV.P(F42:F50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J42" s="7" t="e">
-        <f>I42/SQRT(COUNT(F42:F50))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="7" t="e">
-        <f>AVERAGE(L42:L50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O42" s="7" t="e">
-        <f>_xlfn.STDEV.P(L42:L50)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="P42" s="7" t="e">
-        <f>O42/SQRT(COUNT(L42:L50))</f>
-        <v>#DIV/0!</v>
+      <c r="D42" s="2">
+        <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="2">
         <v>13</v>
       </c>
       <c r="C43" s="2">
         <v>1990.85</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="2"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="8"/>
-      <c r="P43" s="8"/>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B44" s="2">
-        <v>14</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="2"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="8"/>
-      <c r="P44" s="8"/>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B45" s="2">
-        <v>15</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="8"/>
-      <c r="P45" s="8"/>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="8"/>
-      <c r="P46" s="8"/>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="8"/>
-      <c r="P48" s="8"/>
-    </row>
-    <row r="49" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="8"/>
-      <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
-    </row>
-    <row r="50" spans="6:16" x14ac:dyDescent="0.3">
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="9"/>
-      <c r="O50" s="9"/>
-      <c r="P50" s="9"/>
+      <c r="D43" s="2">
+        <v>0.1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="15">
+    <mergeCell ref="Q3:R6"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="J38:J40"/>
+    <mergeCell ref="N31:N33"/>
+    <mergeCell ref="O31:O33"/>
+    <mergeCell ref="P31:P33"/>
+    <mergeCell ref="H31:H34"/>
+    <mergeCell ref="I31:I34"/>
+    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="N37:N39"/>
+    <mergeCell ref="O37:O39"/>
+    <mergeCell ref="P37:P39"/>
+    <mergeCell ref="H38:H40"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="K2:O2"/>
-    <mergeCell ref="H31:H39"/>
-    <mergeCell ref="I31:I39"/>
-    <mergeCell ref="J31:J39"/>
-    <mergeCell ref="P31:P39"/>
-    <mergeCell ref="N42:N50"/>
-    <mergeCell ref="O42:O50"/>
-    <mergeCell ref="P42:P50"/>
-    <mergeCell ref="H42:H50"/>
-    <mergeCell ref="I42:I50"/>
-    <mergeCell ref="J42:J50"/>
-    <mergeCell ref="N31:N39"/>
-    <mergeCell ref="O31:O39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
T4B - Ligeiras melhorias
- alinhar tabelas
- corrigir nota do asterisco
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive - Universidade do Porto\Ambiente de Trabalho\GIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA11C410-C8BE-4E6F-A36F-E778F0AFF54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6B1BFA-A153-4BEE-B9BB-33EEB919F2D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -196,20 +196,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,8 +226,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -244,15 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -273,7 +265,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -340,7 +332,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -531,7 +523,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="368582591"/>
@@ -593,7 +585,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="368580095"/>
@@ -641,7 +633,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -655,7 +647,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -722,7 +714,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -913,7 +905,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="367098383"/>
@@ -975,7 +967,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="367097551"/>
@@ -1023,7 +1015,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2224,7 +2216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2523,38 +2515,38 @@
   <dimension ref="B2:R43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="K2" s="11" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="K2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2573,7 +2565,7 @@
       <c r="H3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="15">
         <v>38.5</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -2591,12 +2583,12 @@
       <c r="O3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q3" s="14" t="s">
+      <c r="Q3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="14"/>
+      <c r="R3" s="11"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -2629,10 +2621,10 @@
         <f>M4-$I$3</f>
         <v>-5.5</v>
       </c>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
@@ -2665,10 +2657,10 @@
         <f t="shared" ref="O5:O12" si="1">M5-$I$3</f>
         <v>-5</v>
       </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
@@ -2701,10 +2693,10 @@
         <f t="shared" si="1"/>
         <v>-4.5</v>
       </c>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
@@ -2737,8 +2729,10 @@
         <f t="shared" si="1"/>
         <v>-4.1000000000000014</v>
       </c>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>19</v>
       </c>
@@ -2771,8 +2765,10 @@
         <f t="shared" si="1"/>
         <v>-3.7000000000000028</v>
       </c>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>20</v>
       </c>
@@ -2807,7 +2803,7 @@
         <v>-3.2999999999999972</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
@@ -2841,7 +2837,7 @@
         <v>-2.2999999999999972</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
@@ -2875,7 +2871,7 @@
         <v>-1.3999999999999986</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
@@ -2909,7 +2905,7 @@
         <v>-0.79999999999999716</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3">
@@ -2918,12 +2914,12 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="I26" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>7</v>
       </c>
@@ -2933,7 +2929,7 @@
       <c r="D30" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="13" t="s">
+      <c r="F30" s="10" t="s">
         <v>27</v>
       </c>
       <c r="G30" s="8" t="s">
@@ -2964,7 +2960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>1</v>
       </c>
@@ -2981,15 +2977,15 @@
         <v>0.01</v>
       </c>
       <c r="H31" s="12">
-        <f>AVERAGE(F31:F36)</f>
+        <f>AVERAGE(F31:F35)</f>
         <v>0.13025</v>
       </c>
       <c r="I31" s="12">
-        <f>_xlfn.STDEV.P(F31:F36)</f>
+        <f>_xlfn.STDEV.P(F31:F35)</f>
         <v>1.4790199457749053E-3</v>
       </c>
       <c r="J31" s="12">
-        <f>I31/SQRT(COUNT(F31:F36))</f>
+        <f>I31/SQRT(COUNT(F31:F35))</f>
         <v>7.3950997288745263E-4</v>
       </c>
       <c r="L31" s="2">
@@ -3011,7 +3007,7 @@
         <v>2.7216552697591257E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
         <v>2</v>
       </c>
@@ -3040,7 +3036,7 @@
       <c r="O32" s="12"/>
       <c r="P32" s="12"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
         <v>3</v>
       </c>
@@ -3069,7 +3065,7 @@
       <c r="O33" s="12"/>
       <c r="P33" s="12"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>4</v>
       </c>
@@ -3089,7 +3085,7 @@
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>5</v>
       </c>
@@ -3100,7 +3096,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>6</v>
       </c>
@@ -3110,6 +3106,21 @@
       <c r="D36" s="2">
         <v>0.1</v>
       </c>
+      <c r="F36" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>13</v>
+      </c>
       <c r="L36" s="8" t="s">
         <v>28</v>
       </c>
@@ -3126,7 +3137,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>7</v>
       </c>
@@ -3136,20 +3147,21 @@
       <c r="D37" s="2">
         <v>0.1</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>13</v>
+      <c r="F37" s="2">
+        <v>252.1</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="12">
+        <f>AVERAGE(F37:F50)</f>
+        <v>251.26666666666665</v>
+      </c>
+      <c r="I37" s="12">
+        <f>_xlfn.STDEV.P(F37:F50)</f>
+        <v>0.69442222186665081</v>
+      </c>
+      <c r="J37" s="12">
+        <f>I37/SQRT(COUNT(F37:F50))</f>
+        <v>0.40092485672596889</v>
       </c>
       <c r="L37" s="2">
         <v>22</v>
@@ -3170,7 +3182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>8</v>
       </c>
@@ -3181,21 +3193,12 @@
         <v>0.1</v>
       </c>
       <c r="F38" s="2">
-        <v>252.1</v>
+        <v>250.4</v>
       </c>
       <c r="G38" s="2"/>
-      <c r="H38" s="12">
-        <f>AVERAGE(F38:F50)</f>
-        <v>251.26666666666665</v>
-      </c>
-      <c r="I38" s="12">
-        <f>_xlfn.STDEV.P(F38:F50)</f>
-        <v>0.69442222186665081</v>
-      </c>
-      <c r="J38" s="12">
-        <f>I38/SQRT(COUNT(F38:F50))</f>
-        <v>0.40092485672596889</v>
-      </c>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
       <c r="L38" s="2">
         <v>22</v>
       </c>
@@ -3206,7 +3209,7 @@
       <c r="O38" s="12"/>
       <c r="P38" s="12"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>9</v>
       </c>
@@ -3217,7 +3220,7 @@
         <v>0.1</v>
       </c>
       <c r="F39" s="2">
-        <v>250.4</v>
+        <v>251.3</v>
       </c>
       <c r="G39" s="2"/>
       <c r="H39" s="12"/>
@@ -3233,7 +3236,7 @@
       <c r="O39" s="12"/>
       <c r="P39" s="12"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>10</v>
       </c>
@@ -3243,20 +3246,13 @@
       <c r="D40" s="2">
         <v>0.1</v>
       </c>
-      <c r="F40" s="2">
-        <v>251.3</v>
-      </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>11</v>
       </c>
@@ -3267,7 +3263,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>12</v>
       </c>
@@ -3278,7 +3274,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>13</v>
       </c>
@@ -3291,21 +3287,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="Q3:R6"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="J38:J40"/>
-    <mergeCell ref="N31:N33"/>
-    <mergeCell ref="O31:O33"/>
-    <mergeCell ref="P31:P33"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q3:R8"/>
     <mergeCell ref="H31:H34"/>
     <mergeCell ref="I31:I34"/>
     <mergeCell ref="J31:J34"/>
     <mergeCell ref="N37:N39"/>
     <mergeCell ref="O37:O39"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="N31:N33"/>
+    <mergeCell ref="O31:O33"/>
+    <mergeCell ref="P31:P33"/>
     <mergeCell ref="P37:P39"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="K2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
T4B - Ligeiras melhorias 2
As mesmas de antes, mas agora deve de funcionar :)
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\OneDrive - Universidade do Porto\Ambiente de Trabalho\GIT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2393CAE0-A49F-4043-A4F0-673D0542A59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE49B27-E808-45F0-9763-4F2B1C1FB0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -196,20 +196,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -235,17 +226,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,6 +238,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -273,7 +265,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -340,7 +332,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -531,7 +523,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="368582591"/>
@@ -593,7 +585,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="368580095"/>
@@ -641,7 +633,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -655,7 +647,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="pt-PT"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -722,7 +714,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pt-PT"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -913,7 +905,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="367098383"/>
@@ -975,7 +967,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pt-PT"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="367097551"/>
@@ -1023,7 +1015,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="pt-PT"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2224,7 +2216,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2522,39 +2514,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83617AA6-E6F3-42B7-BA6C-E56FF542CF9F}">
   <dimension ref="B2:R43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="K2" s="14" t="s">
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="K2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2570,10 +2562,10 @@
       <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="15">
         <v>38.5</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -2591,12 +2583,12 @@
       <c r="O3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="R3" s="11"/>
+      <c r="R3" s="14"/>
     </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -2629,10 +2621,10 @@
         <f>M4-$I$3</f>
         <v>-5.5</v>
       </c>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
@@ -2665,10 +2657,10 @@
         <f t="shared" ref="O5:O12" si="1">M5-$I$3</f>
         <v>-5</v>
       </c>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
@@ -2701,10 +2693,10 @@
         <f t="shared" si="1"/>
         <v>-4.5</v>
       </c>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
@@ -2737,8 +2729,10 @@
         <f t="shared" si="1"/>
         <v>-4.1000000000000014</v>
       </c>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>12</v>
       </c>
@@ -2771,8 +2765,10 @@
         <f t="shared" si="1"/>
         <v>-3.7000000000000028</v>
       </c>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2807,7 +2803,7 @@
         <v>-3.2999999999999972</v>
       </c>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>14</v>
       </c>
@@ -2841,7 +2837,7 @@
         <v>-2.2999999999999972</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
@@ -2875,7 +2871,7 @@
         <v>-1.3999999999999986</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
@@ -2909,7 +2905,7 @@
         <v>-0.79999999999999716</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3">
@@ -2918,12 +2914,12 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="I26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="7" t="s">
         <v>5</v>
       </c>
@@ -2933,7 +2929,7 @@
       <c r="D30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="9" t="s">
         <v>20</v>
       </c>
       <c r="G30" s="8" t="s">
@@ -2964,7 +2960,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>1</v>
       </c>
@@ -2980,16 +2976,16 @@
       <c r="G31" s="2">
         <v>0.01</v>
       </c>
-      <c r="H31" s="12">
-        <f>AVERAGE(F31:F36)</f>
+      <c r="H31" s="13">
+        <f>AVERAGE(F31:F35)</f>
         <v>0.13025</v>
       </c>
-      <c r="I31" s="12">
-        <f>_xlfn.STDEV.P(F31:F36)</f>
+      <c r="I31" s="13">
+        <f>_xlfn.STDEV.P(F31:F35)</f>
         <v>1.4790199457749053E-3</v>
       </c>
-      <c r="J31" s="12">
-        <f>I31/SQRT(COUNT(F31:F36))</f>
+      <c r="J31" s="13">
+        <f>I31/SQRT(COUNT(F31:F35))</f>
         <v>7.3950997288745263E-4</v>
       </c>
       <c r="L31" s="2">
@@ -2998,20 +2994,20 @@
       <c r="M31" s="2">
         <v>0.05</v>
       </c>
-      <c r="N31" s="12">
+      <c r="N31" s="13">
         <f>AVERAGE(L31:L33)</f>
         <v>38.533333333333331</v>
       </c>
-      <c r="O31" s="12">
+      <c r="O31" s="13">
         <f>_xlfn.STDEV.P(L31:L33)</f>
         <v>4.7140452079103841E-2</v>
       </c>
-      <c r="P31" s="12">
+      <c r="P31" s="13">
         <f>O31/SQRT(COUNT(L31:L33))</f>
         <v>2.7216552697591257E-2</v>
       </c>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
         <v>2</v>
       </c>
@@ -3027,20 +3023,20 @@
       <c r="G32" s="2">
         <v>0.01</v>
       </c>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
       <c r="L32" s="2">
         <v>38.6</v>
       </c>
       <c r="M32" s="2">
         <v>0.05</v>
       </c>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="12"/>
+      <c r="N32" s="13"/>
+      <c r="O32" s="13"/>
+      <c r="P32" s="13"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
         <v>3</v>
       </c>
@@ -3056,20 +3052,20 @@
       <c r="G33" s="2">
         <v>0.01</v>
       </c>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
       <c r="L33" s="2">
         <v>38.5</v>
       </c>
       <c r="M33" s="2">
         <v>0.05</v>
       </c>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="12"/>
+      <c r="N33" s="13"/>
+      <c r="O33" s="13"/>
+      <c r="P33" s="13"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>4</v>
       </c>
@@ -3085,11 +3081,11 @@
       <c r="G34" s="2">
         <v>0.01</v>
       </c>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>5</v>
       </c>
@@ -3100,7 +3096,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>6</v>
       </c>
@@ -3110,6 +3106,21 @@
       <c r="D36" s="2">
         <v>0.1</v>
       </c>
+      <c r="F36" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="L36" s="8" t="s">
         <v>21</v>
       </c>
@@ -3126,7 +3137,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>7</v>
       </c>
@@ -3136,20 +3147,21 @@
       <c r="D37" s="2">
         <v>0.1</v>
       </c>
-      <c r="F37" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H37" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J37" s="8" t="s">
-        <v>8</v>
+      <c r="F37" s="2">
+        <v>252.1</v>
+      </c>
+      <c r="G37" s="2"/>
+      <c r="H37" s="13">
+        <f>AVERAGE(F37:F50)</f>
+        <v>251.26666666666665</v>
+      </c>
+      <c r="I37" s="13">
+        <f>_xlfn.STDEV.P(F37:F50)</f>
+        <v>0.69442222186665081</v>
+      </c>
+      <c r="J37" s="13">
+        <f>I37/SQRT(COUNT(F37:F50))</f>
+        <v>0.40092485672596889</v>
       </c>
       <c r="L37" s="2">
         <v>22</v>
@@ -3157,20 +3169,20 @@
       <c r="M37" s="2">
         <v>0.05</v>
       </c>
-      <c r="N37" s="12">
+      <c r="N37" s="13">
         <f>AVERAGE(L37:L50)</f>
         <v>22</v>
       </c>
-      <c r="O37" s="12">
+      <c r="O37" s="13">
         <f>_xlfn.STDEV.P(L37:L50)</f>
         <v>0</v>
       </c>
-      <c r="P37" s="12">
+      <c r="P37" s="13">
         <f>O37/SQRT(COUNT(L37:L50))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>8</v>
       </c>
@@ -3181,32 +3193,23 @@
         <v>0.1</v>
       </c>
       <c r="F38" s="2">
-        <v>252.1</v>
+        <v>250.4</v>
       </c>
       <c r="G38" s="2"/>
-      <c r="H38" s="12">
-        <f>AVERAGE(F38:F50)</f>
-        <v>251.26666666666665</v>
-      </c>
-      <c r="I38" s="12">
-        <f>_xlfn.STDEV.P(F38:F50)</f>
-        <v>0.69442222186665081</v>
-      </c>
-      <c r="J38" s="12">
-        <f>I38/SQRT(COUNT(F38:F50))</f>
-        <v>0.40092485672596889</v>
-      </c>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
       <c r="L38" s="2">
         <v>22</v>
       </c>
       <c r="M38" s="2">
         <v>0.05</v>
       </c>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="12"/>
+      <c r="N38" s="13"/>
+      <c r="O38" s="13"/>
+      <c r="P38" s="13"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>9</v>
       </c>
@@ -3217,23 +3220,23 @@
         <v>0.1</v>
       </c>
       <c r="F39" s="2">
-        <v>250.4</v>
+        <v>251.3</v>
       </c>
       <c r="G39" s="2"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
       <c r="L39" s="2">
         <v>22</v>
       </c>
       <c r="M39" s="2">
         <v>0.05</v>
       </c>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
-      <c r="P39" s="12"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>10</v>
       </c>
@@ -3243,20 +3246,13 @@
       <c r="D40" s="2">
         <v>0.1</v>
       </c>
-      <c r="F40" s="2">
-        <v>251.3</v>
-      </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
       <c r="L40" s="5"/>
       <c r="M40" s="5"/>
       <c r="N40" s="5"/>
       <c r="O40" s="5"/>
       <c r="P40" s="5"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>11</v>
       </c>
@@ -3267,7 +3263,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>12</v>
       </c>
@@ -3278,7 +3274,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>13</v>
       </c>
@@ -3291,21 +3287,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N37:N39"/>
+    <mergeCell ref="O37:O39"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="I37:I39"/>
+    <mergeCell ref="J37:J39"/>
+    <mergeCell ref="N31:N33"/>
+    <mergeCell ref="O31:O33"/>
+    <mergeCell ref="P31:P33"/>
+    <mergeCell ref="P37:P39"/>
+    <mergeCell ref="Q3:R8"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="H31:H34"/>
     <mergeCell ref="I31:I34"/>
     <mergeCell ref="J31:J34"/>
-    <mergeCell ref="N37:N39"/>
-    <mergeCell ref="O37:O39"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="Q3:R6"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="J38:J40"/>
-    <mergeCell ref="N31:N33"/>
-    <mergeCell ref="O31:O33"/>
-    <mergeCell ref="P31:P33"/>
-    <mergeCell ref="P37:P39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
T4B - contas corrigidas e com resíduos
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE49B27-E808-45F0-9763-4F2B1C1FB0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC848BC4-3BEE-405A-84BF-7911CDBBC3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
   <si>
     <t>Carga</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>nº da massa</t>
-  </si>
-  <si>
-    <t>Média</t>
   </si>
   <si>
     <t>Desvio padrão</t>
@@ -91,16 +88,10 @@
     <t>1002.65</t>
   </si>
   <si>
-    <t>L0</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>diametro (φ) (cm)</t>
-  </si>
-  <si>
-    <t>h (cm)</t>
   </si>
   <si>
     <t>u(h) (cm)</t>
@@ -118,12 +109,6 @@
     <t>* Incerteza obtida por cálculo, devido a oscilações no valor apresentado no instrumento de medida.</t>
   </si>
   <si>
-    <t>d(cm)</t>
-  </si>
-  <si>
-    <t>M Carga (g)</t>
-  </si>
-  <si>
     <t>m (g)</t>
   </si>
   <si>
@@ -138,11 +123,45 @@
   <si>
     <t>u(D) (cm)</t>
   </si>
+  <si>
+    <t>Módulo de Young:</t>
+  </si>
+  <si>
+    <t>b (cm)</t>
+  </si>
+  <si>
+    <t>Média (m)</t>
+  </si>
+  <si>
+    <t>M Carga (kg)</t>
+  </si>
+  <si>
+    <t>u(Lc) (m)</t>
+  </si>
+  <si>
+    <t>d(m)</t>
+  </si>
+  <si>
+    <t>Erro percentual:</t>
+  </si>
+  <si>
+    <t>Resíduos</t>
+  </si>
+  <si>
+    <t>Fit</t>
+  </si>
+  <si>
+    <t>L0 (m)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -159,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,8 +191,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -196,20 +221,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -232,19 +280,55 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -296,14 +380,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>massa carga</a:t>
+              <a:rPr lang="en-US" sz="1500"/>
+              <a:t>Massa de carga</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> em func de d (carga)</a:t>
+              <a:rPr lang="en-US" sz="1500" baseline="0"/>
+              <a:t> em função de d (durante a carga)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1500"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -351,7 +435,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>d(cm)</c:v>
+                  <c:v>d(m)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -378,74 +462,130 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.51785731972182725"/>
+                  <c:y val="8.5483012540099157E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$12</c:f>
+              <c:f>Sheet1!$F$4:$F$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.20000000000000284</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.79999999999999716</c:v>
+                  <c:v>2.0000000000000287E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5</c:v>
+                  <c:v>7.9999999999999724E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7000000000000028</c:v>
+                  <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2000000000000028</c:v>
+                  <c:v>1.7000000000000029E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.6000000000000014</c:v>
+                  <c:v>2.200000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1000000000000014</c:v>
+                  <c:v>2.6000000000000016E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.5</c:v>
+                  <c:v>4.1000000000000016E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.5</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$12</c:f>
+              <c:f>Sheet1!$C$4:$C$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2000.75</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3003.4</c:v>
+                  <c:v>2.00075</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4000.4</c:v>
+                  <c:v>3.0034000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5002.1000000000004</c:v>
+                  <c:v>4.0004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6003.3</c:v>
+                  <c:v>5.0021000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6999.6</c:v>
+                  <c:v>6.0033000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7999.15</c:v>
+                  <c:v>6.9996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8996.7000000000007</c:v>
+                  <c:v>7.9991500000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9997.4</c:v>
+                  <c:v>8.9967000000000006</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.9974000000000007</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -489,7 +629,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>d (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -551,7 +746,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>massa de carga(kg)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -678,17 +928,25 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>massa em func de d</a:t>
+              <a:rPr lang="en-US" sz="1500"/>
+              <a:t>Massa de carga em função de d</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> (descarga)</a:t>
+              <a:rPr lang="en-US" sz="1500" baseline="0"/>
+              <a:t> (durante a descarga)</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="1500"/>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16033482464562532"/>
+          <c:y val="3.3055564954556964E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -733,7 +991,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>d(cm)</c:v>
+                  <c:v>d(m)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -760,74 +1018,130 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.19448495099215646"/>
+                  <c:y val="4.5122484689413822E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$4:$O$12</c:f>
+              <c:f>Sheet1!$O$4:$O$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-5.5</c:v>
+                  <c:v>5.5E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4.5</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-4.1000000000000014</c:v>
+                  <c:v>4.1000000000000016E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-3.7000000000000028</c:v>
+                  <c:v>3.7000000000000026E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-3.2999999999999972</c:v>
+                  <c:v>3.2999999999999974E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-2.2999999999999972</c:v>
+                  <c:v>2.2999999999999972E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-1.3999999999999986</c:v>
+                  <c:v>1.3999999999999986E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.79999999999999716</c:v>
+                  <c:v>7.9999999999999724E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.0000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$L$12</c:f>
+              <c:f>Sheet1!$L$4:$L$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9997.4</c:v>
+                  <c:v>9.9974000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8996.7000000000007</c:v>
+                  <c:v>8.9967000000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7999.15</c:v>
+                  <c:v>7.9991500000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6999.6</c:v>
+                  <c:v>6.9996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6003.3</c:v>
+                  <c:v>6.0033000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5002.1000000000004</c:v>
+                  <c:v>5.0021000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4000.4</c:v>
+                  <c:v>4.0004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3003.4</c:v>
+                  <c:v>3.0034000000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2000.75</c:v>
+                  <c:v>2.00075</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -871,7 +1185,71 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                  </a:rPr>
+                  <a:t>d (m)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -909,7 +1287,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="367098383"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
@@ -933,7 +1311,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>massa de carga(kg)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -971,7 +1404,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="367097551"/>
-        <c:crosses val="autoZero"/>
+        <c:crossesAt val="-1.0000000000000002E-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1003,6 +1436,971 @@
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500"/>
+              <a:t>Resíduos Carga</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Resíduos Carga</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$4:$F$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0000000000000287E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.9999999999999724E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7000000000000029E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.200000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6000000000000016E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.1000000000000016E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$54:$D$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-1.5538000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11391957505817363</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11747830023271844</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5.1128187063661734E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61754138799451219</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.78616532563995811</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1164044757563172</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-0.3817737113073445</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.0284561190984789E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-0.71473668590009254</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-ABC1-404E-A521-411A8303879D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1768942559"/>
+        <c:axId val="1768941727"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1768942559"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>d (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1768941727"/>
+        <c:crossesAt val="-2"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1768941727"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Resíduos</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1200"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1768942559"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1500"/>
+              <a:t>Resíduos Descarga</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Resíduos Descarga</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$4:$O$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1000000000000016E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7000000000000026E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.2999999999999974E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.2999999999999972E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3999999999999986E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.9999999999999724E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-5.0000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$54:$E$63</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.5585969792907175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3688517993551983</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.18225661941967886</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.16852952452873993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.5160656684771574</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.86850181242556523</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.24829217229660472</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21442650381945771</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18492228789683618</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.29265482006448029</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4762-4395-93BB-E28A3ADEBE90}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1605321391"/>
+        <c:axId val="1602953663"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1605321391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>d (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1602953663"/>
+        <c:crossesAt val="-1"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1602953663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Resíduos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1605321391"/>
+        <c:crossesAt val="-1.0000000000000002E-2"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1106,6 +2504,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1623,6 +3101,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2144,13 +4654,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2179,14 +4689,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>411480</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2207,6 +4717,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>830580</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51E0D908-B4C9-48B1-844C-381288BC7934}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2823B76D-8298-41E3-8B60-B865A86BF9A4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2512,10 +5094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83617AA6-E6F3-42B7-BA6C-E56FF542CF9F}">
-  <dimension ref="B2:R43"/>
+  <dimension ref="B2:R63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2523,6 +5105,8 @@
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.88671875" customWidth="1"/>
     <col min="10" max="10" width="9.109375" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
@@ -2531,777 +5115,1048 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="K2" s="12" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="K2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
     </row>
     <row r="3" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="N3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="15">
+      <c r="O3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="R3" s="16"/>
+    </row>
+    <row r="4" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13">
+        <v>0</v>
+      </c>
+      <c r="C4" s="23">
+        <v>0</v>
+      </c>
+      <c r="D4" s="23">
         <v>38.5</v>
       </c>
-      <c r="K3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="R3" s="14"/>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>2000.75</v>
-      </c>
-      <c r="D4" s="2">
-        <v>38.299999999999997</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="E4" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="23">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" s="24">
+        <v>9.9974000000000007</v>
+      </c>
+      <c r="M4" s="24">
+        <v>33</v>
+      </c>
+      <c r="N4" s="24">
         <v>0.1</v>
       </c>
-      <c r="F4" s="2">
-        <f>$I$3-D4</f>
-        <v>0.20000000000000284</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="2">
-        <v>9997.4</v>
-      </c>
-      <c r="M4" s="2">
-        <v>33</v>
-      </c>
-      <c r="N4" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O4" s="2">
-        <f>M4-$I$3</f>
-        <v>-5.5</v>
-      </c>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
+      <c r="O4" s="24">
+        <f>($D$4-M4)*0.01</f>
+        <v>5.5E-2</v>
+      </c>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2">
-        <v>3003.4</v>
-      </c>
-      <c r="D5" s="2">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24">
+        <v>2.00075</v>
+      </c>
+      <c r="D5" s="24">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="24">
+        <f>($D$4-D5)*0.01</f>
+        <v>2.0000000000000287E-3</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" s="24">
+        <v>8.9967000000000006</v>
+      </c>
+      <c r="M5" s="24">
+        <v>33.5</v>
+      </c>
+      <c r="N5" s="24">
         <v>0.1</v>
       </c>
-      <c r="F5" s="2">
-        <f t="shared" ref="F5:F12" si="0">$I$3-D5</f>
-        <v>0.79999999999999716</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="2">
-        <v>8996.7000000000007</v>
-      </c>
-      <c r="M5" s="2">
-        <v>33.5</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O5" s="2">
-        <f t="shared" ref="O5:O12" si="1">M5-$I$3</f>
-        <v>-5</v>
-      </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
+      <c r="O5" s="24">
+        <f t="shared" ref="O5:O13" si="0">($D$4-M5)*0.01</f>
+        <v>0.05</v>
+      </c>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2">
-        <v>4000.4</v>
-      </c>
-      <c r="D6" s="2">
-        <v>37</v>
-      </c>
-      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="C6" s="24">
+        <v>3.0034000000000001</v>
+      </c>
+      <c r="D6" s="24">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="E6" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="24">
+        <f t="shared" ref="F6:F13" si="1">($D$4-D6)*0.01</f>
+        <v>7.9999999999999724E-3</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="K6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="24">
+        <v>7.9991500000000002</v>
+      </c>
+      <c r="M6" s="24">
+        <v>34</v>
+      </c>
+      <c r="N6" s="24">
         <v>0.1</v>
       </c>
-      <c r="F6" s="2">
+      <c r="O6" s="24">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" s="2">
-        <v>7999.15</v>
-      </c>
-      <c r="M6" s="2">
-        <v>34</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O6" s="2">
-        <f t="shared" si="1"/>
-        <v>-4.5</v>
-      </c>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="2">
-        <v>5002.1000000000004</v>
-      </c>
-      <c r="D7" s="2">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="E7" s="2">
+        <v>9</v>
+      </c>
+      <c r="C7" s="24">
+        <v>4.0004</v>
+      </c>
+      <c r="D7" s="24">
+        <v>37</v>
+      </c>
+      <c r="E7" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F7" s="24">
+        <f t="shared" si="1"/>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" s="24">
+        <v>6.9996</v>
+      </c>
+      <c r="M7" s="24">
+        <v>34.4</v>
+      </c>
+      <c r="N7" s="24">
         <v>0.1</v>
       </c>
-      <c r="F7" s="2">
+      <c r="O7" s="24">
         <f t="shared" si="0"/>
-        <v>1.7000000000000028</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="2">
-        <v>6999.6</v>
-      </c>
-      <c r="M7" s="2">
-        <v>34.4</v>
-      </c>
-      <c r="N7" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O7" s="2">
-        <f t="shared" si="1"/>
-        <v>-4.1000000000000014</v>
-      </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
+        <v>4.1000000000000016E-2</v>
+      </c>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="2">
-        <v>6003.3</v>
-      </c>
-      <c r="D8" s="2">
-        <v>36.299999999999997</v>
-      </c>
-      <c r="E8" s="2">
+        <v>10</v>
+      </c>
+      <c r="C8" s="24">
+        <v>5.0021000000000004</v>
+      </c>
+      <c r="D8" s="24">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="E8" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="24">
+        <f t="shared" si="1"/>
+        <v>1.7000000000000029E-2</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="24">
+        <v>6.0033000000000003</v>
+      </c>
+      <c r="M8" s="24">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="N8" s="24">
         <v>0.1</v>
       </c>
-      <c r="F8" s="2">
+      <c r="O8" s="24">
         <f t="shared" si="0"/>
-        <v>2.2000000000000028</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L8" s="2">
-        <v>6003.3</v>
-      </c>
-      <c r="M8" s="2">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="N8" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O8" s="2">
-        <f t="shared" si="1"/>
-        <v>-3.7000000000000028</v>
-      </c>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
+        <v>3.7000000000000026E-2</v>
+      </c>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="2">
-        <v>6999.6</v>
-      </c>
-      <c r="D9" s="2">
-        <v>35.9</v>
-      </c>
-      <c r="E9" s="2">
+        <v>11</v>
+      </c>
+      <c r="C9" s="24">
+        <v>6.0033000000000003</v>
+      </c>
+      <c r="D9" s="24">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="E9" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F9" s="24">
+        <f t="shared" si="1"/>
+        <v>2.200000000000003E-2</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="24">
+        <v>5.0021000000000004</v>
+      </c>
+      <c r="M9" s="24">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="N9" s="24">
         <v>0.1</v>
       </c>
-      <c r="F9" s="2">
+      <c r="O9" s="24">
         <f t="shared" si="0"/>
-        <v>2.6000000000000014</v>
-      </c>
-      <c r="H9" s="6"/>
-      <c r="K9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="2">
-        <v>5002.1000000000004</v>
-      </c>
-      <c r="M9" s="2">
-        <v>35.200000000000003</v>
-      </c>
-      <c r="N9" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O9" s="2">
-        <f t="shared" si="1"/>
-        <v>-3.2999999999999972</v>
-      </c>
+        <v>3.2999999999999974E-2</v>
+      </c>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="2">
-        <v>7999.15</v>
-      </c>
-      <c r="D10" s="2">
-        <v>34.4</v>
-      </c>
-      <c r="E10" s="2">
+        <v>12</v>
+      </c>
+      <c r="C10" s="24">
+        <v>6.9996</v>
+      </c>
+      <c r="D10" s="24">
+        <v>35.9</v>
+      </c>
+      <c r="E10" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="24">
+        <f t="shared" si="1"/>
+        <v>2.6000000000000016E-2</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="K10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="24">
+        <v>4.0004</v>
+      </c>
+      <c r="M10" s="24">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="N10" s="24">
         <v>0.1</v>
       </c>
-      <c r="F10" s="2">
+      <c r="O10" s="24">
         <f t="shared" si="0"/>
-        <v>4.1000000000000014</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="2">
-        <v>4000.4</v>
-      </c>
-      <c r="M10" s="2">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="N10" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O10" s="2">
-        <f t="shared" si="1"/>
-        <v>-2.2999999999999972</v>
+        <v>2.2999999999999972E-2</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="2">
-        <v>8996.7000000000007</v>
-      </c>
-      <c r="D11" s="2">
-        <v>34</v>
-      </c>
-      <c r="E11" s="2">
+        <v>13</v>
+      </c>
+      <c r="C11" s="24">
+        <v>7.9991500000000002</v>
+      </c>
+      <c r="D11" s="24">
+        <v>34.4</v>
+      </c>
+      <c r="E11" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F11" s="24">
+        <f t="shared" si="1"/>
+        <v>4.1000000000000016E-2</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L11" s="24">
+        <v>3.0034000000000001</v>
+      </c>
+      <c r="M11" s="24">
+        <v>37.1</v>
+      </c>
+      <c r="N11" s="24">
         <v>0.1</v>
       </c>
-      <c r="F11" s="2">
+      <c r="O11" s="24">
         <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L11" s="2">
-        <v>3003.4</v>
-      </c>
-      <c r="M11" s="2">
-        <v>37.1</v>
-      </c>
-      <c r="N11" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="O11" s="2">
-        <f t="shared" si="1"/>
-        <v>-1.3999999999999986</v>
+        <v>1.3999999999999986E-2</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="2">
-        <v>9997.4</v>
-      </c>
-      <c r="D12" s="2">
-        <v>33</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="0"/>
-        <v>5.5</v>
+        <v>14</v>
+      </c>
+      <c r="C12" s="24">
+        <v>8.9967000000000006</v>
+      </c>
+      <c r="D12" s="24">
+        <v>34</v>
+      </c>
+      <c r="E12" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F12" s="24">
+        <f t="shared" si="1"/>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
-      <c r="L12" s="2">
-        <v>2000.75</v>
-      </c>
-      <c r="M12" s="2">
+      <c r="L12" s="24">
+        <v>2.00075</v>
+      </c>
+      <c r="M12" s="24">
         <v>37.700000000000003</v>
       </c>
-      <c r="N12" s="2">
+      <c r="N12" s="24">
         <v>0.1</v>
       </c>
-      <c r="O12" s="2">
-        <f t="shared" si="1"/>
-        <v>-0.79999999999999716</v>
+      <c r="O12" s="24">
+        <f t="shared" si="0"/>
+        <v>7.9999999999999724E-3</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3">
+      <c r="B13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="24">
+        <v>9.9974000000000007</v>
+      </c>
+      <c r="D13" s="24">
+        <v>33</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.01</v>
+      </c>
+      <c r="F13" s="24">
+        <f t="shared" si="1"/>
+        <v>5.5E-2</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+      <c r="L13" s="24">
+        <v>0</v>
+      </c>
+      <c r="M13" s="24">
         <v>39</v>
       </c>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="N13" s="24">
+        <v>0.1</v>
+      </c>
+      <c r="O13" s="24">
+        <f t="shared" si="0"/>
+        <v>-5.0000000000000001E-3</v>
+      </c>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="I26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="H30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="M30" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P30" s="8" t="s">
-        <v>8</v>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="I27" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B31" s="2">
-        <v>1</v>
-      </c>
-      <c r="C31" s="2">
-        <v>2005.75</v>
-      </c>
-      <c r="D31" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F31" s="2">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="G31" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="H31" s="13">
-        <f>AVERAGE(F31:F35)</f>
-        <v>0.13025</v>
-      </c>
-      <c r="I31" s="13">
-        <f>_xlfn.STDEV.P(F31:F35)</f>
-        <v>1.4790199457749053E-3</v>
-      </c>
-      <c r="J31" s="13">
-        <f>I31/SQRT(COUNT(F31:F35))</f>
-        <v>7.3950997288745263E-4</v>
-      </c>
-      <c r="L31" s="2">
-        <v>38.5</v>
-      </c>
-      <c r="M31" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="N31" s="13">
-        <f>AVERAGE(L31:L33)</f>
-        <v>38.533333333333331</v>
-      </c>
-      <c r="O31" s="13">
-        <f>_xlfn.STDEV.P(L31:L33)</f>
-        <v>4.7140452079103841E-2</v>
-      </c>
-      <c r="P31" s="13">
-        <f>O31/SQRT(COUNT(L31:L33))</f>
-        <v>2.7216552697591257E-2</v>
+      <c r="B31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P31" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
-        <v>2</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="C32" s="22">
+        <v>2005.75</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.1</v>
       </c>
       <c r="F32" s="2">
-        <v>0.128</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="G32" s="2">
         <v>0.01</v>
       </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
+      <c r="H32" s="26">
+        <f>AVERAGE(F32:F36)*0.01</f>
+        <v>1.3025000000000001E-3</v>
+      </c>
+      <c r="I32" s="26">
+        <f>_xlfn.STDEV.P(F32:F35)</f>
+        <v>1.4790199457749053E-3</v>
+      </c>
+      <c r="J32" s="26">
+        <f>I32/SQRT(COUNT(F32:F36))</f>
+        <v>7.3950997288745263E-4</v>
+      </c>
       <c r="L32" s="2">
-        <v>38.6</v>
+        <v>38.5</v>
       </c>
       <c r="M32" s="2">
         <v>0.05</v>
       </c>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
+      <c r="N32" s="26">
+        <f>AVERAGE(L32:L34)*0.01</f>
+        <v>0.38533333333333331</v>
+      </c>
+      <c r="O32" s="26">
+        <f>_xlfn.STDEV.P(L32:L34)</f>
+        <v>4.7140452079103841E-2</v>
+      </c>
+      <c r="P32" s="26">
+        <f>O32/SQRT(COUNT(L32:L34))</f>
+        <v>2.7216552697591257E-2</v>
+      </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
-        <v>3</v>
-      </c>
-      <c r="C33" s="2">
-        <v>997</v>
-      </c>
-      <c r="D33" s="2">
-        <v>0.1</v>
+        <v>2</v>
+      </c>
+      <c r="C33" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="F33" s="2">
-        <v>0.13200000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="G33" s="2">
         <v>0.01</v>
       </c>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
       <c r="L33" s="2">
-        <v>38.5</v>
+        <v>38.6</v>
       </c>
       <c r="M33" s="2">
         <v>0.05</v>
       </c>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
+      <c r="N33" s="26"/>
+      <c r="O33" s="26"/>
+      <c r="P33" s="26"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2">
-        <v>1001.7</v>
+        <v>3</v>
+      </c>
+      <c r="C34" s="22">
+        <v>997</v>
       </c>
       <c r="D34" s="2">
         <v>0.1</v>
       </c>
       <c r="F34" s="2">
-        <v>0.13</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="G34" s="2">
         <v>0.01</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="L34" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N34" s="26"/>
+      <c r="O34" s="26"/>
+      <c r="P34" s="26"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
-        <v>5</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1001.2</v>
+        <v>4</v>
+      </c>
+      <c r="C35" s="22">
+        <v>1001.7</v>
       </c>
       <c r="D35" s="2">
         <v>0.1</v>
       </c>
+      <c r="F35" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
-        <v>6</v>
-      </c>
-      <c r="C36" s="2">
-        <v>996.3</v>
+        <v>5</v>
+      </c>
+      <c r="C36" s="22">
+        <v>1001.2</v>
       </c>
       <c r="D36" s="2">
         <v>0.1</v>
-      </c>
-      <c r="F36" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="H36" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="I36" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="J36" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L36" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="M36" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N36" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="O36" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="P36" s="8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
-        <v>7</v>
-      </c>
-      <c r="C37" s="2">
-        <v>999.55</v>
+        <v>6</v>
+      </c>
+      <c r="C37" s="22">
+        <v>996.3</v>
       </c>
       <c r="D37" s="2">
         <v>0.1</v>
       </c>
-      <c r="F37" s="2">
-        <v>252.1</v>
-      </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="13">
-        <f>AVERAGE(F37:F50)</f>
-        <v>251.26666666666665</v>
-      </c>
-      <c r="I37" s="13">
-        <f>_xlfn.STDEV.P(F37:F50)</f>
-        <v>0.69442222186665081</v>
-      </c>
-      <c r="J37" s="13">
-        <f>I37/SQRT(COUNT(F37:F50))</f>
-        <v>0.40092485672596889</v>
-      </c>
-      <c r="L37" s="2">
-        <v>22</v>
-      </c>
-      <c r="M37" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="N37" s="13">
-        <f>AVERAGE(L37:L50)</f>
-        <v>22</v>
-      </c>
-      <c r="O37" s="13">
-        <f>_xlfn.STDEV.P(L37:L50)</f>
-        <v>0</v>
-      </c>
-      <c r="P37" s="13">
-        <f>O37/SQRT(COUNT(L37:L50))</f>
-        <v>0</v>
+      <c r="F37" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L37" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M37" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="P37" s="7" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
-        <v>8</v>
-      </c>
-      <c r="C38" s="2">
-        <v>997.55</v>
+        <v>7</v>
+      </c>
+      <c r="C38" s="22">
+        <v>999.55</v>
       </c>
       <c r="D38" s="2">
         <v>0.1</v>
       </c>
       <c r="F38" s="2">
-        <v>250.4</v>
-      </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
+        <v>252.1</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="H38" s="25">
+        <f>AVERAGE(F38:F40)*0.01</f>
+        <v>2.5126666666666666</v>
+      </c>
+      <c r="I38" s="25">
+        <f>_xlfn.STDEV.P(F38:F40)</f>
+        <v>0.69442222186665081</v>
+      </c>
+      <c r="J38" s="25">
+        <f>I38/SQRT(COUNT(F38:F49))</f>
+        <v>0.40092485672596889</v>
+      </c>
       <c r="L38" s="2">
-        <v>22</v>
+        <v>7.25</v>
       </c>
       <c r="M38" s="2">
         <v>0.05</v>
       </c>
-      <c r="N38" s="13"/>
-      <c r="O38" s="13"/>
-      <c r="P38" s="13"/>
+      <c r="N38" s="26">
+        <f>AVERAGE(L38:L40)*0.01</f>
+        <v>7.2166666666666657E-2</v>
+      </c>
+      <c r="O38" s="26">
+        <f>_xlfn.STDEV.P(L38:L40)</f>
+        <v>0.1649915822768612</v>
+      </c>
+      <c r="P38" s="26">
+        <f>O38/SQRT(COUNT(L38:L49))</f>
+        <v>7.3786478737262226E-2</v>
+      </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
-        <v>9</v>
-      </c>
-      <c r="C39" s="2">
-        <v>1000.7</v>
+        <v>8</v>
+      </c>
+      <c r="C39" s="22">
+        <v>997.55</v>
       </c>
       <c r="D39" s="2">
         <v>0.1</v>
       </c>
       <c r="F39" s="2">
-        <v>251.3</v>
-      </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
+        <v>250.4</v>
+      </c>
+      <c r="G39" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
       <c r="L39" s="2">
-        <v>22</v>
+        <v>7.4</v>
       </c>
       <c r="M39" s="2">
         <v>0.05</v>
       </c>
-      <c r="N39" s="13"/>
-      <c r="O39" s="13"/>
-      <c r="P39" s="13"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
-        <v>10</v>
-      </c>
-      <c r="C40" s="2">
-        <v>2003.35</v>
+        <v>9</v>
+      </c>
+      <c r="C40" s="22">
+        <v>1000.7</v>
       </c>
       <c r="D40" s="2">
         <v>0.1</v>
       </c>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
-      <c r="P40" s="5"/>
+      <c r="F40" s="2">
+        <v>251.3</v>
+      </c>
+      <c r="G40" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="L40" s="2">
+        <v>7</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
-        <v>11</v>
-      </c>
-      <c r="C41" s="2">
-        <v>1999.1</v>
+        <v>10</v>
+      </c>
+      <c r="C41" s="22">
+        <v>2003.35</v>
       </c>
       <c r="D41" s="2">
         <v>0.1</v>
       </c>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
-        <v>12</v>
-      </c>
-      <c r="C42" s="2">
-        <v>995.9</v>
+        <v>11</v>
+      </c>
+      <c r="C42" s="22">
+        <v>1999.1</v>
       </c>
       <c r="D42" s="2">
         <v>0.1</v>
       </c>
+      <c r="K42" s="5"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
-        <v>13</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1990.85</v>
+        <v>12</v>
+      </c>
+      <c r="C43" s="22">
+        <v>995.9</v>
       </c>
       <c r="D43" s="2">
         <v>0.1</v>
       </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="M43" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
+        <v>13</v>
+      </c>
+      <c r="C44" s="22">
+        <v>1990.85</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="K44" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="L44" s="17">
+        <f>(SLOPE(C4:C13,F4:F13)*8*H38*I3*9.8)/(N38*PI()*H32^2)</f>
+        <v>62171365007.219116</v>
+      </c>
+      <c r="M44" s="17">
+        <f>(SLOPE(L4:L13,O4:O13)*8*H38*I3*9.8)/(N38*PI()*H32^2)</f>
+        <v>60556831264.170845</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="K45" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="L45" s="18">
+        <f>ABS(L44-1.9*100000000000)/(1.9*100000000000)</f>
+        <v>0.67278228943568885</v>
+      </c>
+      <c r="M45" s="18">
+        <f>ABS(M44-1.9*100000000000)/(1.9*100000000000)</f>
+        <v>0.68127983545173243</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C52" s="20"/>
+      <c r="D52" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" s="20"/>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B53" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B54" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F4+1.5538</f>
+        <v>1.5538000000000001</v>
+      </c>
+      <c r="C54" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O4+0.5183</f>
+        <v>9.4388030207092832</v>
+      </c>
+      <c r="D54" s="21">
+        <f>C4-B54</f>
+        <v>-1.5538000000000001</v>
+      </c>
+      <c r="E54" s="21">
+        <f>L4-C54</f>
+        <v>0.5585969792907175</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B55" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F5+1.5538</f>
+        <v>1.8868304249418264</v>
+      </c>
+      <c r="C55" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O5+0.5183</f>
+        <v>8.6278482006448023</v>
+      </c>
+      <c r="D55" s="21">
+        <f>C5-B55</f>
+        <v>0.11391957505817363</v>
+      </c>
+      <c r="E55" s="21">
+        <f>L5-C55</f>
+        <v>0.3688517993551983</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F6+1.5538</f>
+        <v>2.8859216997672816</v>
+      </c>
+      <c r="C56" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O6+0.5183</f>
+        <v>7.8168933805803213</v>
+      </c>
+      <c r="D56" s="21">
+        <f>C6-B56</f>
+        <v>0.11747830023271844</v>
+      </c>
+      <c r="E56" s="21">
+        <f>L6-C56</f>
+        <v>0.18225661941967886</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F7+1.5538</f>
+        <v>4.0515281870636617</v>
+      </c>
+      <c r="C57" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O7+0.5183</f>
+        <v>7.16812952452874</v>
+      </c>
+      <c r="D57" s="21">
+        <f>C7-B57</f>
+        <v>-5.1128187063661734E-2</v>
+      </c>
+      <c r="E57" s="21">
+        <f>L7-C57</f>
+        <v>-0.16852952452873993</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F8+1.5538</f>
+        <v>4.3845586120054882</v>
+      </c>
+      <c r="C58" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O8+0.5183</f>
+        <v>6.5193656684771577</v>
+      </c>
+      <c r="D58" s="21">
+        <f>C8-B58</f>
+        <v>0.61754138799451219</v>
+      </c>
+      <c r="E58" s="21">
+        <f>L8-C58</f>
+        <v>-0.5160656684771574</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F9+1.5538</f>
+        <v>5.2171346743600422</v>
+      </c>
+      <c r="C59" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O9+0.5183</f>
+        <v>5.8706018124255657</v>
+      </c>
+      <c r="D59" s="21">
+        <f>C9-B59</f>
+        <v>0.78616532563995811</v>
+      </c>
+      <c r="E59" s="21">
+        <f>L9-C59</f>
+        <v>-0.86850181242556523</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B60" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F10+1.5538</f>
+        <v>5.8831955242436829</v>
+      </c>
+      <c r="C60" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O10+0.5183</f>
+        <v>4.2486921722966047</v>
+      </c>
+      <c r="D60" s="21">
+        <f>C10-B60</f>
+        <v>1.1164044757563172</v>
+      </c>
+      <c r="E60" s="21">
+        <f>L10-C60</f>
+        <v>-0.24829217229660472</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B61" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F11+1.5538</f>
+        <v>8.3809237113073447</v>
+      </c>
+      <c r="C61" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O11+0.5183</f>
+        <v>2.7889734961805424</v>
+      </c>
+      <c r="D61" s="21">
+        <f>C11-B61</f>
+        <v>-0.3817737113073445</v>
+      </c>
+      <c r="E61" s="21">
+        <f>L11-C61</f>
+        <v>0.21442650381945771</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B62" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F12+1.5538</f>
+        <v>9.0469845611909854</v>
+      </c>
+      <c r="C62" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O12+0.5183</f>
+        <v>1.8158277121031638</v>
+      </c>
+      <c r="D62" s="21">
+        <f>C12-B62</f>
+        <v>-5.0284561190984789E-2</v>
+      </c>
+      <c r="E62" s="21">
+        <f>L12-C62</f>
+        <v>0.18492228789683618</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B63" s="21">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F13+1.5538</f>
+        <v>10.712136685900093</v>
+      </c>
+      <c r="C63" s="21">
+        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O13+0.5183</f>
+        <v>-0.29265482006448029</v>
+      </c>
+      <c r="D63" s="21">
+        <f>C13-B63</f>
+        <v>-0.71473668590009254</v>
+      </c>
+      <c r="E63" s="21">
+        <f>L13-C63</f>
+        <v>0.29265482006448029</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="N37:N39"/>
-    <mergeCell ref="O37:O39"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="I37:I39"/>
-    <mergeCell ref="J37:J39"/>
-    <mergeCell ref="N31:N33"/>
-    <mergeCell ref="O31:O33"/>
-    <mergeCell ref="P31:P33"/>
-    <mergeCell ref="P37:P39"/>
-    <mergeCell ref="Q3:R8"/>
+  <mergeCells count="17">
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="J38:J40"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="P32:P34"/>
+    <mergeCell ref="P38:P40"/>
+    <mergeCell ref="Q3:R9"/>
+    <mergeCell ref="N38:N40"/>
+    <mergeCell ref="O38:O40"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="K2:O2"/>
-    <mergeCell ref="H31:H34"/>
-    <mergeCell ref="I31:I34"/>
-    <mergeCell ref="J31:J34"/>
+    <mergeCell ref="H32:H35"/>
+    <mergeCell ref="I32:I35"/>
+    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="N32:N34"/>
+    <mergeCell ref="O32:O34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
T4B - tabela do b corrigida
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC848BC4-3BEE-405A-84BF-7911CDBBC3AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8721283-9A65-4D33-981F-A89A3AD6D1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>Carga</t>
   </si>
@@ -94,9 +94,6 @@
     <t>diametro (φ) (cm)</t>
   </si>
   <si>
-    <t>u(h) (cm)</t>
-  </si>
-  <si>
     <t>L0 (cm)</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Módulo de Young:</t>
   </si>
   <si>
-    <t>b (cm)</t>
-  </si>
-  <si>
     <t>Média (m)</t>
   </si>
   <si>
@@ -153,16 +147,26 @@
   <si>
     <t>L0 (m)</t>
   </si>
+  <si>
+    <t>b (m)</t>
+  </si>
+  <si>
+    <t>u(h) (m)</t>
+  </si>
+  <si>
+    <t>Coeficiente de Ampliação:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,6 +180,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -251,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -260,9 +270,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -290,20 +297,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -311,24 +324,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5094,16 +5111,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83617AA6-E6F3-42B7-BA6C-E56FF542CF9F}">
-  <dimension ref="B2:R63"/>
+  <dimension ref="B2:R78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I48" sqref="I48"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -5115,48 +5133,48 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="K2" s="15" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="K2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
     </row>
     <row r="3" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="11">
+        <v>32</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="10">
         <v>0.72899999999999998</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M3" s="3" t="s">
         <v>2</v>
@@ -5165,260 +5183,260 @@
         <v>3</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" s="16"/>
+        <v>32</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="23"/>
     </row>
     <row r="4" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13">
+      <c r="B4" s="12">
         <v>0</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="17">
         <v>0</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="17">
         <v>38.5</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="17">
         <v>0.01</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="17">
         <v>0</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="24">
+      <c r="L4" s="18">
         <v>9.9974000000000007</v>
       </c>
-      <c r="M4" s="24">
+      <c r="M4" s="18">
         <v>33</v>
       </c>
-      <c r="N4" s="24">
+      <c r="N4" s="18">
         <v>0.1</v>
       </c>
-      <c r="O4" s="24">
+      <c r="O4" s="18">
         <f>($D$4-M4)*0.01</f>
         <v>5.5E-2</v>
       </c>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="18">
         <v>2.00075</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="18">
         <v>38.299999999999997</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="17">
         <v>0.01</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="18">
         <f>($D$4-D5)*0.01</f>
         <v>2.0000000000000287E-3</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="24">
+      <c r="L5" s="18">
         <v>8.9967000000000006</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="18">
         <v>33.5</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="18">
         <v>0.1</v>
       </c>
-      <c r="O5" s="24">
+      <c r="O5" s="18">
         <f t="shared" ref="O5:O13" si="0">($D$4-M5)*0.01</f>
         <v>0.05</v>
       </c>
-      <c r="Q5" s="16"/>
-      <c r="R5" s="16"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="24">
+      <c r="C6" s="18">
         <v>3.0034000000000001</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="18">
         <v>37.700000000000003</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="17">
         <v>0.01</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="18">
         <f t="shared" ref="F6:F13" si="1">($D$4-D6)*0.01</f>
         <v>7.9999999999999724E-3</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="4"/>
       <c r="K6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L6" s="24">
+      <c r="L6" s="18">
         <v>7.9991500000000002</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M6" s="18">
         <v>34</v>
       </c>
-      <c r="N6" s="24">
+      <c r="N6" s="18">
         <v>0.1</v>
       </c>
-      <c r="O6" s="24">
+      <c r="O6" s="18">
         <f t="shared" si="0"/>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="Q6" s="16"/>
-      <c r="R6" s="16"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="18">
         <v>4.0004</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="18">
         <v>37</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="17">
         <v>0.01</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="18">
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="24">
+      <c r="L7" s="18">
         <v>6.9996</v>
       </c>
-      <c r="M7" s="24">
+      <c r="M7" s="18">
         <v>34.4</v>
       </c>
-      <c r="N7" s="24">
+      <c r="N7" s="18">
         <v>0.1</v>
       </c>
-      <c r="O7" s="24">
+      <c r="O7" s="18">
         <f t="shared" si="0"/>
         <v>4.1000000000000016E-2</v>
       </c>
-      <c r="Q7" s="16"/>
-      <c r="R7" s="16"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="24">
+      <c r="C8" s="18">
         <v>5.0021000000000004</v>
       </c>
-      <c r="D8" s="24">
+      <c r="D8" s="18">
         <v>36.799999999999997</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="17">
         <v>0.01</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="18">
         <f t="shared" si="1"/>
         <v>1.7000000000000029E-2</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="24">
+      <c r="L8" s="18">
         <v>6.0033000000000003</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="18">
         <v>34.799999999999997</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="18">
         <v>0.1</v>
       </c>
-      <c r="O8" s="24">
+      <c r="O8" s="18">
         <f t="shared" si="0"/>
         <v>3.7000000000000026E-2</v>
       </c>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="16"/>
+      <c r="Q8" s="23"/>
+      <c r="R8" s="23"/>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="18">
         <v>6.0033000000000003</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="18">
         <v>36.299999999999997</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="17">
         <v>0.01</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="18">
         <f t="shared" si="1"/>
         <v>2.200000000000003E-2</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="24">
+      <c r="L9" s="18">
         <v>5.0021000000000004</v>
       </c>
-      <c r="M9" s="24">
+      <c r="M9" s="18">
         <v>35.200000000000003</v>
       </c>
-      <c r="N9" s="24">
+      <c r="N9" s="18">
         <v>0.1</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9" s="18">
         <f t="shared" si="0"/>
         <v>3.2999999999999974E-2</v>
       </c>
-      <c r="Q9" s="16"/>
-      <c r="R9" s="16"/>
+      <c r="Q9" s="23"/>
+      <c r="R9" s="23"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="24">
+      <c r="C10" s="18">
         <v>6.9996</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="18">
         <v>35.9</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="17">
         <v>0.01</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="18">
         <f t="shared" si="1"/>
         <v>2.6000000000000016E-2</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="4"/>
       <c r="K10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="24">
+      <c r="L10" s="18">
         <v>4.0004</v>
       </c>
-      <c r="M10" s="24">
+      <c r="M10" s="18">
         <v>36.200000000000003</v>
       </c>
-      <c r="N10" s="24">
+      <c r="N10" s="18">
         <v>0.1</v>
       </c>
-      <c r="O10" s="24">
+      <c r="O10" s="18">
         <f t="shared" si="0"/>
         <v>2.2999999999999972E-2</v>
       </c>
@@ -5427,32 +5445,32 @@
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="18">
         <v>7.9991500000000002</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="18">
         <v>34.4</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="17">
         <v>0.01</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="18">
         <f t="shared" si="1"/>
         <v>4.1000000000000016E-2</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L11" s="24">
+      <c r="L11" s="18">
         <v>3.0034000000000001</v>
       </c>
-      <c r="M11" s="24">
+      <c r="M11" s="18">
         <v>37.1</v>
       </c>
-      <c r="N11" s="24">
+      <c r="N11" s="18">
         <v>0.1</v>
       </c>
-      <c r="O11" s="24">
+      <c r="O11" s="18">
         <f t="shared" si="0"/>
         <v>1.3999999999999986E-2</v>
       </c>
@@ -5461,32 +5479,32 @@
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="24">
+      <c r="C12" s="18">
         <v>8.9967000000000006</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="18">
         <v>34</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="17">
         <v>0.01</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="18">
         <f t="shared" si="1"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="18">
         <v>2.00075</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="18">
         <v>37.700000000000003</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="18">
         <v>0.1</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12" s="18">
         <f t="shared" si="0"/>
         <v>7.9999999999999724E-3</v>
       </c>
@@ -5495,32 +5513,32 @@
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="18">
         <v>9.9974000000000007</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="18">
         <v>33</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="17">
         <v>0.01</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="18">
         <f t="shared" si="1"/>
         <v>5.5E-2</v>
       </c>
-      <c r="K13" s="10">
+      <c r="K13" s="9">
         <v>0</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="18">
         <v>0</v>
       </c>
-      <c r="M13" s="24">
+      <c r="M13" s="18">
         <v>39</v>
       </c>
-      <c r="N13" s="24">
+      <c r="N13" s="18">
         <v>0.1</v>
       </c>
-      <c r="O13" s="24">
+      <c r="O13" s="18">
         <f t="shared" si="0"/>
         <v>-5.0000000000000001E-3</v>
       </c>
@@ -5531,43 +5549,43 @@
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="F31" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F31" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="7" t="s">
+      <c r="H31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L31" s="7" t="s">
+      <c r="L31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M31" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="M31" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O31" s="7" t="s">
+      <c r="N31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O31" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="P31" s="7" t="s">
+      <c r="P31" s="6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -5575,29 +5593,29 @@
       <c r="B32" s="2">
         <v>1</v>
       </c>
-      <c r="C32" s="22">
+      <c r="C32" s="16">
         <v>2005.75</v>
       </c>
       <c r="D32" s="2">
         <v>0.1</v>
       </c>
       <c r="F32" s="2">
-        <v>0.13100000000000001</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="G32" s="2">
         <v>0.01</v>
       </c>
       <c r="H32" s="26">
         <f>AVERAGE(F32:F36)*0.01</f>
-        <v>1.3025000000000001E-3</v>
-      </c>
-      <c r="I32" s="26">
+        <v>8.7000000000000001E-4</v>
+      </c>
+      <c r="I32" s="22">
         <f>_xlfn.STDEV.P(F32:F35)</f>
-        <v>1.4790199457749053E-3</v>
-      </c>
-      <c r="J32" s="26">
+        <v>7.0710678118654816E-4</v>
+      </c>
+      <c r="J32" s="22">
         <f>I32/SQRT(COUNT(F32:F36))</f>
-        <v>7.3950997288745263E-4</v>
+        <v>3.5355339059327408E-4</v>
       </c>
       <c r="L32" s="2">
         <v>38.5</v>
@@ -5605,15 +5623,15 @@
       <c r="M32" s="2">
         <v>0.05</v>
       </c>
-      <c r="N32" s="26">
+      <c r="N32" s="22">
         <f>AVERAGE(L32:L34)*0.01</f>
         <v>0.38533333333333331</v>
       </c>
-      <c r="O32" s="26">
+      <c r="O32" s="22">
         <f>_xlfn.STDEV.P(L32:L34)</f>
         <v>4.7140452079103841E-2</v>
       </c>
-      <c r="P32" s="26">
+      <c r="P32" s="22">
         <f>O32/SQRT(COUNT(L32:L34))</f>
         <v>2.7216552697591257E-2</v>
       </c>
@@ -5622,85 +5640,85 @@
       <c r="B33" s="2">
         <v>2</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="16" t="s">
         <v>16</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F33" s="2">
-        <v>0.128</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="G33" s="2">
         <v>0.01</v>
       </c>
       <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
       <c r="L33" s="2">
         <v>38.6</v>
       </c>
       <c r="M33" s="2">
         <v>0.05</v>
       </c>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
+      <c r="N33" s="22"/>
+      <c r="O33" s="22"/>
+      <c r="P33" s="22"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>3</v>
       </c>
-      <c r="C34" s="22">
+      <c r="C34" s="16">
         <v>997</v>
       </c>
       <c r="D34" s="2">
         <v>0.1</v>
       </c>
       <c r="F34" s="2">
-        <v>0.13200000000000001</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="G34" s="2">
         <v>0.01</v>
       </c>
       <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
       <c r="L34" s="2">
         <v>38.5</v>
       </c>
       <c r="M34" s="2">
         <v>0.05</v>
       </c>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
+      <c r="N34" s="22"/>
+      <c r="O34" s="22"/>
+      <c r="P34" s="22"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>4</v>
       </c>
-      <c r="C35" s="22">
+      <c r="C35" s="16">
         <v>1001.7</v>
       </c>
       <c r="D35" s="2">
         <v>0.1</v>
       </c>
       <c r="F35" s="2">
-        <v>0.13</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="G35" s="2">
         <v>0.01</v>
       </c>
       <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>5</v>
       </c>
-      <c r="C36" s="22">
+      <c r="C36" s="16">
         <v>1001.2</v>
       </c>
       <c r="D36" s="2">
@@ -5711,48 +5729,39 @@
       <c r="B37" s="2">
         <v>6</v>
       </c>
-      <c r="C37" s="22">
+      <c r="C37" s="16">
         <v>996.3</v>
       </c>
       <c r="D37" s="2">
         <v>0.1</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="G37" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="I37" s="7" t="s">
+      <c r="H37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J37" s="7" t="s">
+      <c r="J37" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L37" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="M37" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N37" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="O37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="P37" s="7" t="s">
-        <v>7</v>
+      <c r="L37" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>7</v>
       </c>
-      <c r="C38" s="22">
+      <c r="C38" s="16">
         <v>999.55</v>
       </c>
       <c r="D38" s="2">
@@ -5764,42 +5773,30 @@
       <c r="G38" s="2">
         <v>0.05</v>
       </c>
-      <c r="H38" s="25">
+      <c r="H38" s="19">
         <f>AVERAGE(F38:F40)*0.01</f>
         <v>2.5126666666666666</v>
       </c>
-      <c r="I38" s="25">
+      <c r="I38" s="19">
         <f>_xlfn.STDEV.P(F38:F40)</f>
         <v>0.69442222186665081</v>
       </c>
-      <c r="J38" s="25">
+      <c r="J38" s="19">
         <f>I38/SQRT(COUNT(F38:F49))</f>
         <v>0.40092485672596889</v>
       </c>
-      <c r="L38" s="2">
-        <v>7.25</v>
-      </c>
-      <c r="M38" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="N38" s="26">
-        <f>AVERAGE(L38:L40)*0.01</f>
-        <v>7.2166666666666657E-2</v>
-      </c>
-      <c r="O38" s="26">
-        <f>_xlfn.STDEV.P(L38:L40)</f>
-        <v>0.1649915822768612</v>
-      </c>
-      <c r="P38" s="26">
-        <f>O38/SQRT(COUNT(L38:L49))</f>
-        <v>7.3786478737262226E-2</v>
+      <c r="L38" s="27">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="M38" s="27">
+        <v>5.0000000000000002E-5</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>8</v>
       </c>
-      <c r="C39" s="22">
+      <c r="C39" s="16">
         <v>997.55</v>
       </c>
       <c r="D39" s="2">
@@ -5808,27 +5805,18 @@
       <c r="F39" s="2">
         <v>250.4</v>
       </c>
-      <c r="G39" s="10">
+      <c r="G39" s="9">
         <v>0.05</v>
       </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="L39" s="2">
-        <v>7.4</v>
-      </c>
-      <c r="M39" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="N39" s="26"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="26"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>9</v>
       </c>
-      <c r="C40" s="22">
+      <c r="C40" s="16">
         <v>1000.7</v>
       </c>
       <c r="D40" s="2">
@@ -5837,65 +5825,59 @@
       <c r="F40" s="2">
         <v>251.3</v>
       </c>
-      <c r="G40" s="10">
+      <c r="G40" s="9">
         <v>0.05</v>
       </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="L40" s="2">
-        <v>7</v>
-      </c>
-      <c r="M40" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>10</v>
       </c>
-      <c r="C41" s="22">
+      <c r="C41" s="16">
         <v>2003.35</v>
       </c>
       <c r="D41" s="2">
         <v>0.1</v>
       </c>
-      <c r="L41" s="4"/>
-      <c r="M41" s="4"/>
-      <c r="N41" s="4"/>
-      <c r="O41" s="4"/>
-      <c r="P41" s="4"/>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>11</v>
       </c>
-      <c r="C42" s="22">
+      <c r="C42" s="16">
         <v>1999.1</v>
       </c>
       <c r="D42" s="2">
         <v>0.1</v>
       </c>
-      <c r="K42" s="5"/>
+      <c r="K42" s="4"/>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>12</v>
       </c>
-      <c r="C43" s="22">
+      <c r="C43" s="16">
         <v>995.9</v>
       </c>
       <c r="D43" s="2">
         <v>0.1</v>
       </c>
-      <c r="K43" s="5"/>
-      <c r="L43" s="12" t="s">
+      <c r="F43" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="G43" s="24"/>
+      <c r="H43" s="28">
+        <f>2*H38/L38</f>
+        <v>67.909909909909913</v>
+      </c>
+      <c r="K43" s="4"/>
+      <c r="L43" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M43" s="12" t="s">
+      <c r="M43" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5903,253 +5885,306 @@
       <c r="B44" s="2">
         <v>13</v>
       </c>
-      <c r="C44" s="22">
+      <c r="C44" s="16">
         <v>1990.85</v>
       </c>
       <c r="D44" s="2">
         <v>0.1</v>
       </c>
-      <c r="K44" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="L44" s="17">
-        <f>(SLOPE(C4:C13,F4:F13)*8*H38*I3*9.8)/(N38*PI()*H32^2)</f>
-        <v>62171365007.219116</v>
-      </c>
-      <c r="M44" s="17">
-        <f>(SLOPE(L4:L13,O4:O13)*8*H38*I3*9.8)/(N38*PI()*H32^2)</f>
-        <v>60556831264.170845</v>
+      <c r="K44" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="L44" s="13">
+        <f>(SLOPE(C4:C13,F4:F13)*8*H38*I3*9.8)/(L38*PI()*H32^2)</f>
+        <v>135897756643.09407</v>
+      </c>
+      <c r="M44" s="13">
+        <f>(SLOPE(L4:L13,O4:O13)*8*H38*I3*9.8)/(L38*PI()*H32^2)</f>
+        <v>132368615636.1472</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="K45" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="L45" s="18">
+      <c r="K45" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="L45" s="14">
         <f>ABS(L44-1.9*100000000000)/(1.9*100000000000)</f>
-        <v>0.67278228943568885</v>
-      </c>
-      <c r="M45" s="18">
+        <v>0.28474864924687332</v>
+      </c>
+      <c r="M45" s="14">
         <f>ABS(M44-1.9*100000000000)/(1.9*100000000000)</f>
-        <v>0.68127983545173243</v>
+        <v>0.30332307559922528</v>
       </c>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C52" s="20"/>
-      <c r="D52" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" s="20"/>
+      <c r="B52" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C52" s="21"/>
+      <c r="D52" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="E52" s="21"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="12" t="s">
+      <c r="B53" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E53" s="12" t="s">
+      <c r="E53" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F4+1.5538</f>
+      <c r="B54" s="15">
+        <f t="shared" ref="B54:B63" si="2">SLOPE($C$4:$C$13,$F$4:$F$13)*F4+1.5538</f>
         <v>1.5538000000000001</v>
       </c>
-      <c r="C54" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O4+0.5183</f>
+      <c r="C54" s="15">
+        <f t="shared" ref="C54:C63" si="3">SLOPE($L$4:$L$13,$O$4:$O$13)*O4+0.5183</f>
         <v>9.4388030207092832</v>
       </c>
-      <c r="D54" s="21">
-        <f>C4-B54</f>
+      <c r="D54" s="15">
+        <f t="shared" ref="D54:D63" si="4">C4-B54</f>
         <v>-1.5538000000000001</v>
       </c>
-      <c r="E54" s="21">
-        <f>L4-C54</f>
+      <c r="E54" s="15">
+        <f t="shared" ref="E54:E63" si="5">L4-C54</f>
         <v>0.5585969792907175</v>
       </c>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F5+1.5538</f>
+      <c r="B55" s="15">
+        <f t="shared" si="2"/>
         <v>1.8868304249418264</v>
       </c>
-      <c r="C55" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O5+0.5183</f>
+      <c r="C55" s="15">
+        <f t="shared" si="3"/>
         <v>8.6278482006448023</v>
       </c>
-      <c r="D55" s="21">
-        <f>C5-B55</f>
+      <c r="D55" s="15">
+        <f t="shared" si="4"/>
         <v>0.11391957505817363</v>
       </c>
-      <c r="E55" s="21">
-        <f>L5-C55</f>
+      <c r="E55" s="15">
+        <f t="shared" si="5"/>
         <v>0.3688517993551983</v>
       </c>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F6+1.5538</f>
+      <c r="B56" s="15">
+        <f t="shared" si="2"/>
         <v>2.8859216997672816</v>
       </c>
-      <c r="C56" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O6+0.5183</f>
+      <c r="C56" s="15">
+        <f t="shared" si="3"/>
         <v>7.8168933805803213</v>
       </c>
-      <c r="D56" s="21">
-        <f>C6-B56</f>
+      <c r="D56" s="15">
+        <f t="shared" si="4"/>
         <v>0.11747830023271844</v>
       </c>
-      <c r="E56" s="21">
-        <f>L6-C56</f>
+      <c r="E56" s="15">
+        <f t="shared" si="5"/>
         <v>0.18225661941967886</v>
       </c>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F7+1.5538</f>
+      <c r="B57" s="15">
+        <f t="shared" si="2"/>
         <v>4.0515281870636617</v>
       </c>
-      <c r="C57" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O7+0.5183</f>
+      <c r="C57" s="15">
+        <f t="shared" si="3"/>
         <v>7.16812952452874</v>
       </c>
-      <c r="D57" s="21">
-        <f>C7-B57</f>
+      <c r="D57" s="15">
+        <f t="shared" si="4"/>
         <v>-5.1128187063661734E-2</v>
       </c>
-      <c r="E57" s="21">
-        <f>L7-C57</f>
+      <c r="E57" s="15">
+        <f t="shared" si="5"/>
         <v>-0.16852952452873993</v>
       </c>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F8+1.5538</f>
+      <c r="B58" s="15">
+        <f t="shared" si="2"/>
         <v>4.3845586120054882</v>
       </c>
-      <c r="C58" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O8+0.5183</f>
+      <c r="C58" s="15">
+        <f t="shared" si="3"/>
         <v>6.5193656684771577</v>
       </c>
-      <c r="D58" s="21">
-        <f>C8-B58</f>
+      <c r="D58" s="15">
+        <f t="shared" si="4"/>
         <v>0.61754138799451219</v>
       </c>
-      <c r="E58" s="21">
-        <f>L8-C58</f>
+      <c r="E58" s="15">
+        <f t="shared" si="5"/>
         <v>-0.5160656684771574</v>
       </c>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F9+1.5538</f>
+      <c r="B59" s="15">
+        <f t="shared" si="2"/>
         <v>5.2171346743600422</v>
       </c>
-      <c r="C59" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O9+0.5183</f>
+      <c r="C59" s="15">
+        <f t="shared" si="3"/>
         <v>5.8706018124255657</v>
       </c>
-      <c r="D59" s="21">
-        <f>C9-B59</f>
+      <c r="D59" s="15">
+        <f t="shared" si="4"/>
         <v>0.78616532563995811</v>
       </c>
-      <c r="E59" s="21">
-        <f>L9-C59</f>
+      <c r="E59" s="15">
+        <f t="shared" si="5"/>
         <v>-0.86850181242556523</v>
       </c>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F10+1.5538</f>
+      <c r="B60" s="15">
+        <f t="shared" si="2"/>
         <v>5.8831955242436829</v>
       </c>
-      <c r="C60" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O10+0.5183</f>
+      <c r="C60" s="15">
+        <f t="shared" si="3"/>
         <v>4.2486921722966047</v>
       </c>
-      <c r="D60" s="21">
-        <f>C10-B60</f>
+      <c r="D60" s="15">
+        <f t="shared" si="4"/>
         <v>1.1164044757563172</v>
       </c>
-      <c r="E60" s="21">
-        <f>L10-C60</f>
+      <c r="E60" s="15">
+        <f t="shared" si="5"/>
         <v>-0.24829217229660472</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F11+1.5538</f>
+      <c r="B61" s="15">
+        <f t="shared" si="2"/>
         <v>8.3809237113073447</v>
       </c>
-      <c r="C61" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O11+0.5183</f>
+      <c r="C61" s="15">
+        <f t="shared" si="3"/>
         <v>2.7889734961805424</v>
       </c>
-      <c r="D61" s="21">
-        <f>C11-B61</f>
+      <c r="D61" s="15">
+        <f t="shared" si="4"/>
         <v>-0.3817737113073445</v>
       </c>
-      <c r="E61" s="21">
-        <f>L11-C61</f>
+      <c r="E61" s="15">
+        <f t="shared" si="5"/>
         <v>0.21442650381945771</v>
       </c>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F12+1.5538</f>
+      <c r="B62" s="15">
+        <f t="shared" si="2"/>
         <v>9.0469845611909854</v>
       </c>
-      <c r="C62" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O12+0.5183</f>
+      <c r="C62" s="15">
+        <f t="shared" si="3"/>
         <v>1.8158277121031638</v>
       </c>
-      <c r="D62" s="21">
-        <f>C12-B62</f>
+      <c r="D62" s="15">
+        <f t="shared" si="4"/>
         <v>-5.0284561190984789E-2</v>
       </c>
-      <c r="E62" s="21">
-        <f>L12-C62</f>
+      <c r="E62" s="15">
+        <f t="shared" si="5"/>
         <v>0.18492228789683618</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="21">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F13+1.5538</f>
+      <c r="B63" s="15">
+        <f t="shared" si="2"/>
         <v>10.712136685900093</v>
       </c>
-      <c r="C63" s="21">
-        <f>SLOPE($L$4:$L$13,$O$4:$O$13)*O13+0.5183</f>
+      <c r="C63" s="15">
+        <f t="shared" si="3"/>
         <v>-0.29265482006448029</v>
       </c>
-      <c r="D63" s="21">
-        <f>C13-B63</f>
+      <c r="D63" s="15">
+        <f t="shared" si="4"/>
         <v>-0.71473668590009254</v>
       </c>
-      <c r="E63" s="21">
-        <f>L13-C63</f>
+      <c r="E63" s="15">
+        <f t="shared" si="5"/>
         <v>0.29265482006448029</v>
       </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="D68" s="29"/>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C69" s="30"/>
+      <c r="D69" s="31"/>
+      <c r="E69" s="31"/>
+      <c r="F69" s="31"/>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="30"/>
+      <c r="D70" s="31"/>
+      <c r="E70" s="31"/>
+      <c r="F70" s="31"/>
+    </row>
+    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C71" s="30"/>
+      <c r="D71" s="31"/>
+      <c r="E71" s="31"/>
+      <c r="F71" s="31"/>
+    </row>
+    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C72" s="30"/>
+      <c r="D72" s="31"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
+    </row>
+    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C73" s="30"/>
+      <c r="D73" s="31"/>
+      <c r="E73" s="31"/>
+      <c r="F73" s="31"/>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C74" s="30"/>
+      <c r="D74" s="31"/>
+      <c r="E74" s="31"/>
+      <c r="F74" s="31"/>
+    </row>
+    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C75" s="30"/>
+      <c r="D75" s="31"/>
+      <c r="E75" s="31"/>
+      <c r="F75" s="31"/>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C76" s="30"/>
+      <c r="D76" s="31"/>
+      <c r="E76" s="31"/>
+      <c r="F76" s="31"/>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C77" s="30"/>
+      <c r="D77" s="31"/>
+      <c r="E77" s="31"/>
+      <c r="F77" s="31"/>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C78" s="30"/>
+      <c r="D78" s="31"/>
+      <c r="E78" s="31"/>
+      <c r="F78" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="J38:J40"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="P32:P34"/>
-    <mergeCell ref="P38:P40"/>
-    <mergeCell ref="Q3:R9"/>
-    <mergeCell ref="N38:N40"/>
-    <mergeCell ref="O38:O40"/>
+  <mergeCells count="15">
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="H32:H35"/>
@@ -6157,8 +6192,17 @@
     <mergeCell ref="J32:J35"/>
     <mergeCell ref="N32:N34"/>
     <mergeCell ref="O32:O34"/>
+    <mergeCell ref="P32:P34"/>
+    <mergeCell ref="Q3:R9"/>
+    <mergeCell ref="H38:H40"/>
+    <mergeCell ref="I38:I40"/>
+    <mergeCell ref="J38:J40"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F43:G43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
T4B - pronto a imprimir
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8721283-9A65-4D33-981F-A89A3AD6D1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4530078-FED2-440E-9732-CC055C0B4E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
@@ -166,7 +166,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,12 +180,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -208,7 +202,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -257,11 +251,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,6 +322,28 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -324,28 +353,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,7 +1014,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$3</c:f>
+              <c:f>Sheet1!$N$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1087,7 +1097,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$4:$O$13</c:f>
+              <c:f>Sheet1!$N$4:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1126,7 +1136,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$L$13</c:f>
+              <c:f>Sheet1!$K$4:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1620,7 +1630,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$54:$D$63</c:f>
+              <c:f>Sheet1!$O$38:$O$47</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2064,7 +2074,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$O$4:$O$13</c:f>
+              <c:f>Sheet1!$N$4:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2103,7 +2113,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$54:$E$63</c:f>
+              <c:f>Sheet1!$P$38:$P$47</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -4741,16 +4751,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>35411</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>62753</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>830580</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>857474</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>62753</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4777,16 +4787,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>35859</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>358140</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>483646</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5111,10 +5121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83617AA6-E6F3-42B7-BA6C-E56FF542CF9F}">
-  <dimension ref="B2:R78"/>
+  <dimension ref="B2:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5122,33 +5132,34 @@
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="4" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.109375" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="10" max="10" width="17.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" customWidth="1"/>
     <col min="12" max="12" width="12.5546875" customWidth="1"/>
     <col min="15" max="15" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="K2" s="25" t="s">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="J2" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
     </row>
-    <row r="3" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -5167,30 +5178,27 @@
       <c r="H3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="10">
-        <v>0.72899999999999998</v>
+      <c r="J3" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="23" t="s">
+      <c r="P3" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="R3" s="23"/>
+      <c r="Q3" s="26"/>
     </row>
-    <row r="4" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="12">
         <v>0</v>
       </c>
@@ -5206,26 +5214,29 @@
       <c r="F4" s="17">
         <v>0</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="H4" s="10">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="K4" s="18">
+        <v>9.9974000000000007</v>
+      </c>
       <c r="L4" s="18">
-        <v>9.9974000000000007</v>
+        <v>33</v>
       </c>
       <c r="M4" s="18">
-        <v>33</v>
+        <v>0.1</v>
       </c>
       <c r="N4" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O4" s="18">
-        <f>($D$4-M4)*0.01</f>
+        <f>($D$4-L4)*0.01</f>
         <v>5.5E-2</v>
       </c>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>1</v>
       </c>
@@ -5242,26 +5253,26 @@
         <f>($D$4-D5)*0.01</f>
         <v>2.0000000000000287E-3</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="K5" s="18">
+        <v>8.9967000000000006</v>
+      </c>
       <c r="L5" s="18">
-        <v>8.9967000000000006</v>
+        <v>33.5</v>
       </c>
       <c r="M5" s="18">
-        <v>33.5</v>
+        <v>0.1</v>
       </c>
       <c r="N5" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O5" s="18">
-        <f t="shared" ref="O5:O13" si="0">($D$4-M5)*0.01</f>
+        <f t="shared" ref="N5:N13" si="0">($D$4-L5)*0.01</f>
         <v>0.05</v>
       </c>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -5279,26 +5290,26 @@
         <v>7.9999999999999724E-3</v>
       </c>
       <c r="H6" s="4"/>
-      <c r="K6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="K6" s="18">
+        <v>7.9991500000000002</v>
+      </c>
       <c r="L6" s="18">
-        <v>7.9991500000000002</v>
+        <v>34</v>
       </c>
       <c r="M6" s="18">
-        <v>34</v>
+        <v>0.1</v>
       </c>
       <c r="N6" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O6" s="18">
         <f t="shared" si="0"/>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
@@ -5315,26 +5326,26 @@
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="K7" s="18">
+        <v>6.9996</v>
+      </c>
       <c r="L7" s="18">
-        <v>6.9996</v>
+        <v>34.4</v>
       </c>
       <c r="M7" s="18">
-        <v>34.4</v>
+        <v>0.1</v>
       </c>
       <c r="N7" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O7" s="18">
         <f t="shared" si="0"/>
         <v>4.1000000000000016E-2</v>
       </c>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
     </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
@@ -5351,26 +5362,26 @@
         <f t="shared" si="1"/>
         <v>1.7000000000000029E-2</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="K8" s="18">
+        <v>6.0033000000000003</v>
+      </c>
       <c r="L8" s="18">
-        <v>6.0033000000000003</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="M8" s="18">
-        <v>34.799999999999997</v>
+        <v>0.1</v>
       </c>
       <c r="N8" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O8" s="18">
         <f t="shared" si="0"/>
         <v>3.7000000000000026E-2</v>
       </c>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
     </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
@@ -5387,26 +5398,26 @@
         <f t="shared" si="1"/>
         <v>2.200000000000003E-2</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="K9" s="18">
+        <v>5.0021000000000004</v>
+      </c>
       <c r="L9" s="18">
-        <v>5.0021000000000004</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="M9" s="18">
-        <v>35.200000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="N9" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O9" s="18">
         <f t="shared" si="0"/>
         <v>3.2999999999999974E-2</v>
       </c>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
@@ -5424,24 +5435,24 @@
         <v>2.6000000000000016E-2</v>
       </c>
       <c r="H10" s="4"/>
-      <c r="K10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K10" s="18">
+        <v>4.0004</v>
+      </c>
       <c r="L10" s="18">
-        <v>4.0004</v>
+        <v>36.200000000000003</v>
       </c>
       <c r="M10" s="18">
-        <v>36.200000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="N10" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O10" s="18">
         <f t="shared" si="0"/>
         <v>2.2999999999999972E-2</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
@@ -5458,24 +5469,24 @@
         <f t="shared" si="1"/>
         <v>4.1000000000000016E-2</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="K11" s="18">
+        <v>3.0034000000000001</v>
+      </c>
       <c r="L11" s="18">
-        <v>3.0034000000000001</v>
+        <v>37.1</v>
       </c>
       <c r="M11" s="18">
-        <v>37.1</v>
+        <v>0.1</v>
       </c>
       <c r="N11" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O11" s="18">
         <f t="shared" si="0"/>
         <v>1.3999999999999986E-2</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
@@ -5492,24 +5503,24 @@
         <f t="shared" si="1"/>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="K12" s="2">
+      <c r="J12" s="2">
         <v>1</v>
       </c>
+      <c r="K12" s="18">
+        <v>2.00075</v>
+      </c>
       <c r="L12" s="18">
-        <v>2.00075</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="M12" s="18">
-        <v>37.700000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="N12" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O12" s="18">
         <f t="shared" si="0"/>
         <v>7.9999999999999724E-3</v>
       </c>
     </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
@@ -5526,19 +5537,19 @@
         <f t="shared" si="1"/>
         <v>5.5E-2</v>
       </c>
-      <c r="K13" s="9">
+      <c r="J13" s="9">
         <v>0</v>
       </c>
+      <c r="K13" s="18">
+        <v>0</v>
+      </c>
       <c r="L13" s="18">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="M13" s="18">
-        <v>39</v>
+        <v>0.1</v>
       </c>
       <c r="N13" s="18">
-        <v>0.1</v>
-      </c>
-      <c r="O13" s="18">
         <f t="shared" si="0"/>
         <v>-5.0000000000000001E-3</v>
       </c>
@@ -5549,29 +5560,26 @@
       </c>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B31" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G31" s="6" t="s">
+      <c r="C31" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="H31" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>29</v>
       </c>
+      <c r="E31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="I31" s="6" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="L31" s="6" t="s">
         <v>19</v>
@@ -5590,32 +5598,29 @@
       </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="2">
-        <v>1</v>
-      </c>
-      <c r="C32" s="16">
-        <v>2005.75</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F32" s="2">
+      <c r="B32" s="9">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="G32" s="2">
+      <c r="C32" s="9">
         <v>0.01</v>
       </c>
-      <c r="H32" s="26">
-        <f>AVERAGE(F32:F36)*0.01</f>
+      <c r="D32" s="24">
+        <f>AVERAGE(B32:B36)*0.01</f>
         <v>8.7000000000000001E-4</v>
       </c>
-      <c r="I32" s="22">
-        <f>_xlfn.STDEV.P(F32:F35)</f>
+      <c r="E32" s="25">
+        <f>_xlfn.STDEV.P(B32:B35)</f>
         <v>7.0710678118654816E-4</v>
       </c>
-      <c r="J32" s="22">
-        <f>I32/SQRT(COUNT(F32:F36))</f>
+      <c r="F32" s="25">
+        <f>E32/SQRT(COUNT(B32:B36))</f>
         <v>3.5355339059327408E-4</v>
+      </c>
+      <c r="I32" s="20">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="J32" s="20">
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="L32" s="2">
         <v>38.5</v>
@@ -5623,585 +5628,485 @@
       <c r="M32" s="2">
         <v>0.05</v>
       </c>
-      <c r="N32" s="22">
+      <c r="N32" s="25">
         <f>AVERAGE(L32:L34)*0.01</f>
         <v>0.38533333333333331</v>
       </c>
-      <c r="O32" s="22">
+      <c r="O32" s="25">
         <f>_xlfn.STDEV.P(L32:L34)</f>
         <v>4.7140452079103841E-2</v>
       </c>
-      <c r="P32" s="22">
+      <c r="P32" s="25">
         <f>O32/SQRT(COUNT(L32:L34))</f>
         <v>2.7216552697591257E-2</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B33" s="2">
-        <v>2</v>
-      </c>
-      <c r="C33" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="2">
+      <c r="B33" s="9">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="G33" s="2">
+      <c r="C33" s="9">
         <v>0.01</v>
       </c>
-      <c r="H33" s="26"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
       <c r="L33" s="2">
         <v>38.6</v>
       </c>
       <c r="M33" s="2">
         <v>0.05</v>
       </c>
-      <c r="N33" s="22"/>
-      <c r="O33" s="22"/>
-      <c r="P33" s="22"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="2">
-        <v>3</v>
-      </c>
-      <c r="C34" s="16">
-        <v>997</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F34" s="2">
+      <c r="B34" s="9">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="G34" s="2">
+      <c r="C34" s="9">
         <v>0.01</v>
       </c>
-      <c r="H34" s="26"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
       <c r="L34" s="2">
         <v>38.5</v>
       </c>
       <c r="M34" s="2">
         <v>0.05</v>
       </c>
-      <c r="N34" s="22"/>
-      <c r="O34" s="22"/>
-      <c r="P34" s="22"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35" s="2">
-        <v>4</v>
-      </c>
-      <c r="C35" s="16">
-        <v>1001.7</v>
-      </c>
-      <c r="D35" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F35" s="2">
+      <c r="B35" s="9">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="G35" s="2">
+      <c r="C35" s="9">
         <v>0.01</v>
       </c>
-      <c r="H35" s="26"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
+      <c r="D35" s="24"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B36" s="2">
+      <c r="I36" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="16">
-        <v>1001.2</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.1</v>
-      </c>
+      <c r="J36" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M36" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N36" s="29"/>
+      <c r="O36" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="P36" s="29"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B37" s="2">
+      <c r="B37" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E37" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C37" s="16">
-        <v>996.3</v>
-      </c>
-      <c r="D37" s="2">
+      <c r="F37" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="2">
+        <v>1</v>
+      </c>
+      <c r="J37" s="16">
+        <v>2005.75</v>
+      </c>
+      <c r="K37" s="2">
         <v>0.1</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>38</v>
+      <c r="M37" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="N37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="O37" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P37" s="11" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B38" s="2">
-        <v>7</v>
-      </c>
-      <c r="C38" s="16">
-        <v>999.55</v>
-      </c>
-      <c r="D38" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F38" s="2">
+      <c r="B38" s="9">
         <v>252.1</v>
       </c>
-      <c r="G38" s="2">
+      <c r="C38" s="9">
         <v>0.05</v>
       </c>
-      <c r="H38" s="19">
-        <f>AVERAGE(F38:F40)*0.01</f>
+      <c r="D38" s="27">
+        <f>AVERAGE(B38:B40)*0.01</f>
         <v>2.5126666666666666</v>
       </c>
-      <c r="I38" s="19">
-        <f>_xlfn.STDEV.P(F38:F40)</f>
+      <c r="E38" s="27">
+        <f>_xlfn.STDEV.P(B38:B40)</f>
         <v>0.69442222186665081</v>
       </c>
-      <c r="J38" s="19">
-        <f>I38/SQRT(COUNT(F38:F49))</f>
-        <v>0.40092485672596889</v>
-      </c>
-      <c r="L38" s="27">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="M38" s="27">
-        <v>5.0000000000000002E-5</v>
+      <c r="F38" s="27" t="e">
+        <f>E38/SQRT(COUNT(F49:F49))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I38" s="2">
+        <v>2</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M38" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F4+1.5538</f>
+        <v>1.5538000000000001</v>
+      </c>
+      <c r="N38" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N4+0.5183</f>
+        <v>9.4388030207092832</v>
+      </c>
+      <c r="O38" s="15">
+        <f>C4-M38</f>
+        <v>-1.5538000000000001</v>
+      </c>
+      <c r="P38" s="15">
+        <f>K4-N38</f>
+        <v>0.5585969792907175</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B39" s="2">
-        <v>8</v>
-      </c>
-      <c r="C39" s="16">
-        <v>997.55</v>
-      </c>
-      <c r="D39" s="2">
+      <c r="B39" s="9">
+        <v>250.4</v>
+      </c>
+      <c r="C39" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="I39" s="2">
+        <v>3</v>
+      </c>
+      <c r="J39" s="16">
+        <v>997</v>
+      </c>
+      <c r="K39" s="2">
         <v>0.1</v>
       </c>
-      <c r="F39" s="2">
-        <v>250.4</v>
-      </c>
-      <c r="G39" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
-      <c r="J39" s="19"/>
+      <c r="M39" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F5+1.5538</f>
+        <v>1.8868304249418264</v>
+      </c>
+      <c r="N39" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N5+0.5183</f>
+        <v>8.6278482006448023</v>
+      </c>
+      <c r="O39" s="15">
+        <f>C5-M39</f>
+        <v>0.11391957505817363</v>
+      </c>
+      <c r="P39" s="15">
+        <f>K5-N39</f>
+        <v>0.3688517993551983</v>
+      </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B40" s="2">
-        <v>9</v>
-      </c>
-      <c r="C40" s="16">
-        <v>1000.7</v>
-      </c>
-      <c r="D40" s="2">
+      <c r="B40" s="9">
+        <v>251.3</v>
+      </c>
+      <c r="C40" s="9">
+        <v>0.05</v>
+      </c>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
+      <c r="I40" s="2">
+        <v>4</v>
+      </c>
+      <c r="J40" s="16">
+        <v>1001.7</v>
+      </c>
+      <c r="K40" s="2">
         <v>0.1</v>
       </c>
-      <c r="F40" s="2">
-        <v>251.3</v>
-      </c>
-      <c r="G40" s="9">
-        <v>0.05</v>
-      </c>
-      <c r="H40" s="19"/>
-      <c r="I40" s="19"/>
-      <c r="J40" s="19"/>
+      <c r="M40" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F6+1.5538</f>
+        <v>2.8859216997672816</v>
+      </c>
+      <c r="N40" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N6+0.5183</f>
+        <v>7.8168933805803213</v>
+      </c>
+      <c r="O40" s="15">
+        <f>C6-M40</f>
+        <v>0.11747830023271844</v>
+      </c>
+      <c r="P40" s="15">
+        <f>K6-N40</f>
+        <v>0.18225661941967886</v>
+      </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B41" s="2">
-        <v>10</v>
-      </c>
-      <c r="C41" s="16">
-        <v>2003.35</v>
-      </c>
-      <c r="D41" s="2">
+      <c r="I41" s="2">
+        <v>5</v>
+      </c>
+      <c r="J41" s="16">
+        <v>1001.2</v>
+      </c>
+      <c r="K41" s="2">
         <v>0.1</v>
+      </c>
+      <c r="M41" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F7+1.5538</f>
+        <v>4.0515281870636617</v>
+      </c>
+      <c r="N41" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N7+0.5183</f>
+        <v>7.16812952452874</v>
+      </c>
+      <c r="O41" s="15">
+        <f>C7-M41</f>
+        <v>-5.1128187063661734E-2</v>
+      </c>
+      <c r="P41" s="15">
+        <f>K7-N41</f>
+        <v>-0.16852952452873993</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B42" s="2">
-        <v>11</v>
-      </c>
-      <c r="C42" s="16">
-        <v>1999.1</v>
-      </c>
-      <c r="D42" s="2">
+      <c r="I42" s="2">
+        <v>6</v>
+      </c>
+      <c r="J42" s="16">
+        <v>996.3</v>
+      </c>
+      <c r="K42" s="2">
         <v>0.1</v>
       </c>
-      <c r="K42" s="4"/>
+      <c r="M42" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F8+1.5538</f>
+        <v>4.3845586120054882</v>
+      </c>
+      <c r="N42" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N8+0.5183</f>
+        <v>6.5193656684771577</v>
+      </c>
+      <c r="O42" s="15">
+        <f>C8-M42</f>
+        <v>0.61754138799451219</v>
+      </c>
+      <c r="P42" s="15">
+        <f>K8-N42</f>
+        <v>-0.5160656684771574</v>
+      </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B43" s="2">
-        <v>12</v>
-      </c>
-      <c r="C43" s="16">
-        <v>995.9</v>
-      </c>
-      <c r="D43" s="2">
+      <c r="B43" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="C43" s="29"/>
+      <c r="D43" s="21">
+        <f>2*D38/I32</f>
+        <v>67.909909909909913</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="I43" s="2">
+        <v>7</v>
+      </c>
+      <c r="J43" s="16">
+        <v>999.55</v>
+      </c>
+      <c r="K43" s="2">
         <v>0.1</v>
       </c>
-      <c r="F43" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="G43" s="24"/>
-      <c r="H43" s="28">
-        <f>2*H38/L38</f>
-        <v>67.909909909909913</v>
-      </c>
-      <c r="K43" s="4"/>
-      <c r="L43" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="M43" s="11" t="s">
-        <v>4</v>
+      <c r="M43" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F9+1.5538</f>
+        <v>5.2171346743600422</v>
+      </c>
+      <c r="N43" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N9+0.5183</f>
+        <v>5.8706018124255657</v>
+      </c>
+      <c r="O43" s="15">
+        <f>C9-M43</f>
+        <v>0.78616532563995811</v>
+      </c>
+      <c r="P43" s="15">
+        <f>K9-N43</f>
+        <v>-0.86850181242556523</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B44" s="2">
-        <v>13</v>
-      </c>
-      <c r="C44" s="16">
-        <v>1990.85</v>
-      </c>
-      <c r="D44" s="2">
+      <c r="E44" s="4"/>
+      <c r="F44" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="I44" s="2">
+        <v>8</v>
+      </c>
+      <c r="J44" s="16">
+        <v>997.55</v>
+      </c>
+      <c r="K44" s="2">
         <v>0.1</v>
       </c>
-      <c r="K44" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L44" s="13">
-        <f>(SLOPE(C4:C13,F4:F13)*8*H38*I3*9.8)/(L38*PI()*H32^2)</f>
-        <v>135897756643.09407</v>
-      </c>
-      <c r="M44" s="13">
-        <f>(SLOPE(L4:L13,O4:O13)*8*H38*I3*9.8)/(L38*PI()*H32^2)</f>
-        <v>132368615636.1472</v>
+      <c r="M44" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F10+1.5538</f>
+        <v>5.8831955242436829</v>
+      </c>
+      <c r="N44" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N10+0.5183</f>
+        <v>4.2486921722966047</v>
+      </c>
+      <c r="O44" s="15">
+        <f>C10-M44</f>
+        <v>1.1164044757563172</v>
+      </c>
+      <c r="P44" s="15">
+        <f>K10-N44</f>
+        <v>-0.24829217229660472</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="K45" s="11" t="s">
+      <c r="D45" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="22"/>
+      <c r="F45" s="13">
+        <f>(SLOPE(C4:C13,F4:F13)*8*D38*H4*9.8)/(I32*PI()*D32^2)</f>
+        <v>135897756643.09407</v>
+      </c>
+      <c r="G45" s="13">
+        <f>(SLOPE(K4:K13,N4:N13)*8*D38*H4*9.8)/(I32*PI()*D32^2)</f>
+        <v>132368615636.1472</v>
+      </c>
+      <c r="I45" s="2">
+        <v>9</v>
+      </c>
+      <c r="J45" s="16">
+        <v>1000.7</v>
+      </c>
+      <c r="K45" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M45" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F11+1.5538</f>
+        <v>8.3809237113073447</v>
+      </c>
+      <c r="N45" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N11+0.5183</f>
+        <v>2.7889734961805424</v>
+      </c>
+      <c r="O45" s="15">
+        <f>C11-M45</f>
+        <v>-0.3817737113073445</v>
+      </c>
+      <c r="P45" s="15">
+        <f>K11-N45</f>
+        <v>0.21442650381945771</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D46" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="L45" s="14">
-        <f>ABS(L44-1.9*100000000000)/(1.9*100000000000)</f>
+      <c r="E46" s="22"/>
+      <c r="F46" s="14">
+        <f>ABS(F45-1.9*100000000000)/(1.9*100000000000)</f>
         <v>0.28474864924687332</v>
       </c>
-      <c r="M45" s="14">
-        <f>ABS(M44-1.9*100000000000)/(1.9*100000000000)</f>
+      <c r="G46" s="14">
+        <f>ABS(G45-1.9*100000000000)/(1.9*100000000000)</f>
         <v>0.30332307559922528</v>
       </c>
+      <c r="I46" s="2">
+        <v>10</v>
+      </c>
+      <c r="J46" s="16">
+        <v>2003.35</v>
+      </c>
+      <c r="K46" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M46" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F12+1.5538</f>
+        <v>9.0469845611909854</v>
+      </c>
+      <c r="N46" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N12+0.5183</f>
+        <v>1.8158277121031638</v>
+      </c>
+      <c r="O46" s="15">
+        <f>C12-M46</f>
+        <v>-5.0284561190984789E-2</v>
+      </c>
+      <c r="P46" s="15">
+        <f>K12-N46</f>
+        <v>0.18492228789683618</v>
+      </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B52" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="21"/>
-      <c r="D52" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E52" s="21"/>
-    </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B53" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D53" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B54" s="15">
-        <f t="shared" ref="B54:B63" si="2">SLOPE($C$4:$C$13,$F$4:$F$13)*F4+1.5538</f>
-        <v>1.5538000000000001</v>
-      </c>
-      <c r="C54" s="15">
-        <f t="shared" ref="C54:C63" si="3">SLOPE($L$4:$L$13,$O$4:$O$13)*O4+0.5183</f>
-        <v>9.4388030207092832</v>
-      </c>
-      <c r="D54" s="15">
-        <f t="shared" ref="D54:D63" si="4">C4-B54</f>
-        <v>-1.5538000000000001</v>
-      </c>
-      <c r="E54" s="15">
-        <f t="shared" ref="E54:E63" si="5">L4-C54</f>
-        <v>0.5585969792907175</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B55" s="15">
-        <f t="shared" si="2"/>
-        <v>1.8868304249418264</v>
-      </c>
-      <c r="C55" s="15">
-        <f t="shared" si="3"/>
-        <v>8.6278482006448023</v>
-      </c>
-      <c r="D55" s="15">
-        <f t="shared" si="4"/>
-        <v>0.11391957505817363</v>
-      </c>
-      <c r="E55" s="15">
-        <f t="shared" si="5"/>
-        <v>0.3688517993551983</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B56" s="15">
-        <f t="shared" si="2"/>
-        <v>2.8859216997672816</v>
-      </c>
-      <c r="C56" s="15">
-        <f t="shared" si="3"/>
-        <v>7.8168933805803213</v>
-      </c>
-      <c r="D56" s="15">
-        <f t="shared" si="4"/>
-        <v>0.11747830023271844</v>
-      </c>
-      <c r="E56" s="15">
-        <f t="shared" si="5"/>
-        <v>0.18225661941967886</v>
-      </c>
-    </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B57" s="15">
-        <f t="shared" si="2"/>
-        <v>4.0515281870636617</v>
-      </c>
-      <c r="C57" s="15">
-        <f t="shared" si="3"/>
-        <v>7.16812952452874</v>
-      </c>
-      <c r="D57" s="15">
-        <f t="shared" si="4"/>
-        <v>-5.1128187063661734E-2</v>
-      </c>
-      <c r="E57" s="15">
-        <f t="shared" si="5"/>
-        <v>-0.16852952452873993</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B58" s="15">
-        <f t="shared" si="2"/>
-        <v>4.3845586120054882</v>
-      </c>
-      <c r="C58" s="15">
-        <f t="shared" si="3"/>
-        <v>6.5193656684771577</v>
-      </c>
-      <c r="D58" s="15">
-        <f t="shared" si="4"/>
-        <v>0.61754138799451219</v>
-      </c>
-      <c r="E58" s="15">
-        <f t="shared" si="5"/>
-        <v>-0.5160656684771574</v>
-      </c>
-    </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B59" s="15">
-        <f t="shared" si="2"/>
-        <v>5.2171346743600422</v>
-      </c>
-      <c r="C59" s="15">
-        <f t="shared" si="3"/>
-        <v>5.8706018124255657</v>
-      </c>
-      <c r="D59" s="15">
-        <f t="shared" si="4"/>
-        <v>0.78616532563995811</v>
-      </c>
-      <c r="E59" s="15">
-        <f t="shared" si="5"/>
-        <v>-0.86850181242556523</v>
-      </c>
-    </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B60" s="15">
-        <f t="shared" si="2"/>
-        <v>5.8831955242436829</v>
-      </c>
-      <c r="C60" s="15">
-        <f t="shared" si="3"/>
-        <v>4.2486921722966047</v>
-      </c>
-      <c r="D60" s="15">
-        <f t="shared" si="4"/>
-        <v>1.1164044757563172</v>
-      </c>
-      <c r="E60" s="15">
-        <f t="shared" si="5"/>
-        <v>-0.24829217229660472</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B61" s="15">
-        <f t="shared" si="2"/>
-        <v>8.3809237113073447</v>
-      </c>
-      <c r="C61" s="15">
-        <f t="shared" si="3"/>
-        <v>2.7889734961805424</v>
-      </c>
-      <c r="D61" s="15">
-        <f t="shared" si="4"/>
-        <v>-0.3817737113073445</v>
-      </c>
-      <c r="E61" s="15">
-        <f t="shared" si="5"/>
-        <v>0.21442650381945771</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B62" s="15">
-        <f t="shared" si="2"/>
-        <v>9.0469845611909854</v>
-      </c>
-      <c r="C62" s="15">
-        <f t="shared" si="3"/>
-        <v>1.8158277121031638</v>
-      </c>
-      <c r="D62" s="15">
-        <f t="shared" si="4"/>
-        <v>-5.0284561190984789E-2</v>
-      </c>
-      <c r="E62" s="15">
-        <f t="shared" si="5"/>
-        <v>0.18492228789683618</v>
-      </c>
-    </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B63" s="15">
-        <f t="shared" si="2"/>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="M47" s="15">
+        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F13+1.5538</f>
         <v>10.712136685900093</v>
       </c>
-      <c r="C63" s="15">
-        <f t="shared" si="3"/>
+      <c r="N47" s="15">
+        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N13+0.5183</f>
         <v>-0.29265482006448029</v>
       </c>
-      <c r="D63" s="15">
-        <f t="shared" si="4"/>
+      <c r="O47" s="15">
+        <f>C13-M47</f>
         <v>-0.71473668590009254</v>
       </c>
-      <c r="E63" s="15">
-        <f t="shared" si="5"/>
+      <c r="P47" s="15">
+        <f>K13-N47</f>
         <v>0.29265482006448029</v>
       </c>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="D68" s="29"/>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C69" s="30"/>
-      <c r="D69" s="31"/>
-      <c r="E69" s="31"/>
-      <c r="F69" s="31"/>
-    </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C70" s="30"/>
-      <c r="D70" s="31"/>
-      <c r="E70" s="31"/>
-      <c r="F70" s="31"/>
-    </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C71" s="30"/>
-      <c r="D71" s="31"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-    </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C72" s="30"/>
-      <c r="D72" s="31"/>
-      <c r="E72" s="31"/>
-      <c r="F72" s="31"/>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C73" s="30"/>
-      <c r="D73" s="31"/>
-      <c r="E73" s="31"/>
-      <c r="F73" s="31"/>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C74" s="30"/>
-      <c r="D74" s="31"/>
-      <c r="E74" s="31"/>
-      <c r="F74" s="31"/>
-    </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C75" s="30"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="31"/>
-      <c r="F75" s="31"/>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C76" s="30"/>
-      <c r="D76" s="31"/>
-      <c r="E76" s="31"/>
-      <c r="F76" s="31"/>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C77" s="30"/>
-      <c r="D77" s="31"/>
-      <c r="E77" s="31"/>
-      <c r="F77" s="31"/>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.3">
-      <c r="C78" s="30"/>
-      <c r="D78" s="31"/>
-      <c r="E78" s="31"/>
-      <c r="F78" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="P32:P34"/>
+    <mergeCell ref="P3:Q9"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
     <mergeCell ref="B2:F2"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="H32:H35"/>
-    <mergeCell ref="I32:I35"/>
-    <mergeCell ref="J32:J35"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
     <mergeCell ref="N32:N34"/>
     <mergeCell ref="O32:O34"/>
-    <mergeCell ref="P32:P34"/>
-    <mergeCell ref="Q3:R9"/>
-    <mergeCell ref="H38:H40"/>
-    <mergeCell ref="I38:I40"/>
-    <mergeCell ref="J38:J40"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F43:G43"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>

<commit_message>
T4B - Versão mesmo final
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4530078-FED2-440E-9732-CC055C0B4E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B85112D-1167-4D91-A1FD-F77C2B0EC6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Carga</t>
   </si>
@@ -92,12 +92,6 @@
   </si>
   <si>
     <t>diametro (φ) (cm)</t>
-  </si>
-  <si>
-    <t>L0 (cm)</t>
-  </si>
-  <si>
-    <t>u(L0) (cm)</t>
   </si>
   <si>
     <t>0,15*</t>
@@ -268,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -291,13 +285,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -329,14 +319,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -347,13 +340,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4679,16 +4672,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>189412</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>18506</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>854530</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>18506</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4715,16 +4708,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7619</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>734785</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5123,8 +5116,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83617AA6-E6F3-42B7-BA6C-E56FF542CF9F}">
   <dimension ref="B2:Q47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5144,45 +5137,42 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="J2" s="23" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="J2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
     </row>
     <row r="3" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>2</v>
@@ -5191,101 +5181,98 @@
         <v>3</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" s="26"/>
+        <v>30</v>
+      </c>
+      <c r="P3" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="25"/>
     </row>
     <row r="4" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="12">
+      <c r="B4" s="10">
         <v>0</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="15">
         <v>0</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="15">
         <v>38.5</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="15">
         <v>0.01</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="15">
         <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0.72899999999999998</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="16">
         <v>9.9974000000000007</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="16">
         <v>33</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="16">
         <v>0.1</v>
       </c>
-      <c r="N4" s="18">
+      <c r="N4" s="16">
         <f>($D$4-L4)*0.01</f>
         <v>5.5E-2</v>
       </c>
-      <c r="P4" s="26"/>
-      <c r="Q4" s="26"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>2.00075</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <v>38.299999999999997</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="15">
         <v>0.01</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="16">
         <f>($D$4-D5)*0.01</f>
         <v>2.0000000000000287E-3</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="16">
         <v>8.9967000000000006</v>
       </c>
-      <c r="L5" s="18">
+      <c r="L5" s="16">
         <v>33.5</v>
       </c>
-      <c r="M5" s="18">
+      <c r="M5" s="16">
         <v>0.1</v>
       </c>
-      <c r="N5" s="18">
+      <c r="N5" s="16">
         <f t="shared" ref="N5:N13" si="0">($D$4-L5)*0.01</f>
         <v>0.05</v>
       </c>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>3.0034000000000001</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <v>37.700000000000003</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="15">
         <v>0.01</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="16">
         <f t="shared" ref="F6:F13" si="1">($D$4-D6)*0.01</f>
         <v>7.9999999999999724E-3</v>
       </c>
@@ -5293,144 +5280,144 @@
       <c r="J6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="16">
         <v>7.9991500000000002</v>
       </c>
-      <c r="L6" s="18">
+      <c r="L6" s="16">
         <v>34</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="16">
         <v>0.1</v>
       </c>
-      <c r="N6" s="18">
+      <c r="N6" s="16">
         <f t="shared" si="0"/>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="P6" s="26"/>
-      <c r="Q6" s="26"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="16">
         <v>4.0004</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>37</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="15">
         <v>0.01</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="16">
         <f t="shared" si="1"/>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="16">
         <v>6.9996</v>
       </c>
-      <c r="L7" s="18">
+      <c r="L7" s="16">
         <v>34.4</v>
       </c>
-      <c r="M7" s="18">
+      <c r="M7" s="16">
         <v>0.1</v>
       </c>
-      <c r="N7" s="18">
+      <c r="N7" s="16">
         <f t="shared" si="0"/>
         <v>4.1000000000000016E-2</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="16">
         <v>5.0021000000000004</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="16">
         <v>36.799999999999997</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="15">
         <v>0.01</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="16">
         <f t="shared" si="1"/>
         <v>1.7000000000000029E-2</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="16">
         <v>6.0033000000000003</v>
       </c>
-      <c r="L8" s="18">
+      <c r="L8" s="16">
         <v>34.799999999999997</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="16">
         <v>0.1</v>
       </c>
-      <c r="N8" s="18">
+      <c r="N8" s="16">
         <f t="shared" si="0"/>
         <v>3.7000000000000026E-2</v>
       </c>
-      <c r="P8" s="26"/>
-      <c r="Q8" s="26"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="16">
         <v>6.0033000000000003</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <v>36.299999999999997</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="15">
         <v>0.01</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="16">
         <f t="shared" si="1"/>
         <v>2.200000000000003E-2</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="16">
         <v>5.0021000000000004</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="16">
         <v>35.200000000000003</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="16">
         <v>0.1</v>
       </c>
-      <c r="N9" s="18">
+      <c r="N9" s="16">
         <f t="shared" si="0"/>
         <v>3.2999999999999974E-2</v>
       </c>
-      <c r="P9" s="26"/>
-      <c r="Q9" s="26"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="16">
         <v>6.9996</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <v>35.9</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="15">
         <v>0.01</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="16">
         <f t="shared" si="1"/>
         <v>2.6000000000000016E-2</v>
       </c>
@@ -5438,16 +5425,16 @@
       <c r="J10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="16">
         <v>4.0004</v>
       </c>
-      <c r="L10" s="18">
+      <c r="L10" s="16">
         <v>36.200000000000003</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="16">
         <v>0.1</v>
       </c>
-      <c r="N10" s="18">
+      <c r="N10" s="16">
         <f t="shared" si="0"/>
         <v>2.2999999999999972E-2</v>
       </c>
@@ -5456,32 +5443,32 @@
       <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="16">
         <v>7.9991500000000002</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <v>34.4</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="15">
         <v>0.01</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="16">
         <f t="shared" si="1"/>
         <v>4.1000000000000016E-2</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="16">
         <v>3.0034000000000001</v>
       </c>
-      <c r="L11" s="18">
+      <c r="L11" s="16">
         <v>37.1</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="16">
         <v>0.1</v>
       </c>
-      <c r="N11" s="18">
+      <c r="N11" s="16">
         <f t="shared" si="0"/>
         <v>1.3999999999999986E-2</v>
       </c>
@@ -5490,32 +5477,32 @@
       <c r="B12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="16">
         <v>8.9967000000000006</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <v>34</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="15">
         <v>0.01</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="16">
         <f t="shared" si="1"/>
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="J12" s="2">
         <v>1</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="16">
         <v>2.00075</v>
       </c>
-      <c r="L12" s="18">
+      <c r="L12" s="16">
         <v>37.700000000000003</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="16">
         <v>0.1</v>
       </c>
-      <c r="N12" s="18">
+      <c r="N12" s="16">
         <f t="shared" si="0"/>
         <v>7.9999999999999724E-3</v>
       </c>
@@ -5524,50 +5511,50 @@
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="16">
         <v>9.9974000000000007</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <v>33</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="15">
         <v>0.01</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="16">
         <f t="shared" si="1"/>
         <v>5.5E-2</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <v>0</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="16">
         <v>0</v>
       </c>
-      <c r="L13" s="18">
+      <c r="L13" s="16">
         <v>39</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="16">
         <v>0.1</v>
       </c>
-      <c r="N13" s="18">
+      <c r="N13" s="16">
         <f t="shared" si="0"/>
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
       <c r="I27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B31" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="19" t="s">
-        <v>25</v>
+      <c r="C31" s="17" t="s">
+        <v>23</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>6</v>
@@ -5576,150 +5563,107 @@
         <v>7</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="O31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P31" s="6" t="s">
-        <v>7</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="L31" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M31" s="23"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="9">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="8">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>0.01</v>
       </c>
-      <c r="D32" s="24">
+      <c r="D32" s="28">
         <f>AVERAGE(B32:B36)*0.01</f>
         <v>8.7000000000000001E-4</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="24">
         <f>_xlfn.STDEV.P(B32:B35)</f>
         <v>7.0710678118654816E-4</v>
       </c>
-      <c r="F32" s="25">
+      <c r="F32" s="24">
         <f>E32/SQRT(COUNT(B32:B36))</f>
         <v>3.5355339059327408E-4</v>
       </c>
-      <c r="I32" s="20">
+      <c r="I32" s="18">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="J32" s="20">
+      <c r="J32" s="18">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="L32" s="2">
-        <v>38.5</v>
-      </c>
-      <c r="M32" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="N32" s="25">
-        <f>AVERAGE(L32:L34)*0.01</f>
-        <v>0.38533333333333331</v>
-      </c>
-      <c r="O32" s="25">
-        <f>_xlfn.STDEV.P(L32:L34)</f>
-        <v>4.7140452079103841E-2</v>
-      </c>
-      <c r="P32" s="25">
-        <f>O32/SQRT(COUNT(L32:L34))</f>
-        <v>2.7216552697591257E-2</v>
-      </c>
+      <c r="L32" s="29">
+        <v>0.72899999999999998</v>
+      </c>
+      <c r="M32" s="29"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B33" s="9">
+      <c r="B33" s="8">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="8">
         <v>0.01</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="L33" s="2">
-        <v>38.6</v>
-      </c>
-      <c r="M33" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="9">
+      <c r="B34" s="8">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="8">
         <v>0.01</v>
       </c>
-      <c r="D34" s="24"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="L34" s="2">
-        <v>38.5</v>
-      </c>
-      <c r="M34" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35" s="9">
+      <c r="B35" s="8">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <v>0.01</v>
       </c>
-      <c r="D35" s="24"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="24"/>
+      <c r="F35" s="24"/>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="I36" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M36" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="N36" s="29"/>
-      <c r="O36" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="P36" s="29"/>
+        <v>22</v>
+      </c>
+      <c r="M36" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="N36" s="22"/>
+      <c r="O36" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="P36" s="22"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B37" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="19" t="s">
+      <c r="B37" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D37" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>6</v>
@@ -5730,139 +5674,139 @@
       <c r="I37" s="2">
         <v>1</v>
       </c>
-      <c r="J37" s="16">
+      <c r="J37" s="14">
         <v>2005.75</v>
       </c>
       <c r="K37" s="2">
         <v>0.1</v>
       </c>
-      <c r="M37" s="11" t="s">
+      <c r="M37" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="N37" s="11" t="s">
+      <c r="N37" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="O37" s="11" t="s">
+      <c r="O37" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="P37" s="11" t="s">
+      <c r="P37" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B38" s="9">
+      <c r="B38" s="8">
         <v>252.1</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8">
         <v>0.05</v>
       </c>
-      <c r="D38" s="27">
+      <c r="D38" s="26">
         <f>AVERAGE(B38:B40)*0.01</f>
         <v>2.5126666666666666</v>
       </c>
-      <c r="E38" s="27">
+      <c r="E38" s="26">
         <f>_xlfn.STDEV.P(B38:B40)</f>
         <v>0.69442222186665081</v>
       </c>
-      <c r="F38" s="27" t="e">
-        <f>E38/SQRT(COUNT(F49:F49))</f>
-        <v>#DIV/0!</v>
+      <c r="F38" s="26">
+        <f>E38/SQRT(3)</f>
+        <v>0.40092485672596889</v>
       </c>
       <c r="I38" s="2">
         <v>2</v>
       </c>
-      <c r="J38" s="16" t="s">
+      <c r="J38" s="14" t="s">
         <v>16</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M38" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F4+1.5538</f>
+        <v>19</v>
+      </c>
+      <c r="M38" s="13">
+        <f t="shared" ref="M38:M47" si="2">SLOPE($C$4:$C$13,$F$4:$F$13)*F4+1.5538</f>
         <v>1.5538000000000001</v>
       </c>
-      <c r="N38" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N4+0.5183</f>
+      <c r="N38" s="13">
+        <f t="shared" ref="N38:N47" si="3">SLOPE($K$4:$K$13,$N$4:$N$13)*N4+0.5183</f>
         <v>9.4388030207092832</v>
       </c>
-      <c r="O38" s="15">
-        <f>C4-M38</f>
+      <c r="O38" s="13">
+        <f t="shared" ref="O38:O47" si="4">C4-M38</f>
         <v>-1.5538000000000001</v>
       </c>
-      <c r="P38" s="15">
-        <f>K4-N38</f>
+      <c r="P38" s="13">
+        <f t="shared" ref="P38:P47" si="5">K4-N38</f>
         <v>0.5585969792907175</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B39" s="9">
+      <c r="B39" s="8">
         <v>250.4</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="8">
         <v>0.05</v>
       </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
       <c r="I39" s="2">
         <v>3</v>
       </c>
-      <c r="J39" s="16">
+      <c r="J39" s="14">
         <v>997</v>
       </c>
       <c r="K39" s="2">
         <v>0.1</v>
       </c>
-      <c r="M39" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F5+1.5538</f>
+      <c r="M39" s="13">
+        <f t="shared" si="2"/>
         <v>1.8868304249418264</v>
       </c>
-      <c r="N39" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N5+0.5183</f>
+      <c r="N39" s="13">
+        <f t="shared" si="3"/>
         <v>8.6278482006448023</v>
       </c>
-      <c r="O39" s="15">
-        <f>C5-M39</f>
+      <c r="O39" s="13">
+        <f t="shared" si="4"/>
         <v>0.11391957505817363</v>
       </c>
-      <c r="P39" s="15">
-        <f>K5-N39</f>
+      <c r="P39" s="13">
+        <f t="shared" si="5"/>
         <v>0.3688517993551983</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B40" s="9">
+      <c r="B40" s="8">
         <v>251.3</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="8">
         <v>0.05</v>
       </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
       <c r="I40" s="2">
         <v>4</v>
       </c>
-      <c r="J40" s="16">
+      <c r="J40" s="14">
         <v>1001.7</v>
       </c>
       <c r="K40" s="2">
         <v>0.1</v>
       </c>
-      <c r="M40" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F6+1.5538</f>
+      <c r="M40" s="13">
+        <f t="shared" si="2"/>
         <v>2.8859216997672816</v>
       </c>
-      <c r="N40" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N6+0.5183</f>
+      <c r="N40" s="13">
+        <f t="shared" si="3"/>
         <v>7.8168933805803213</v>
       </c>
-      <c r="O40" s="15">
-        <f>C6-M40</f>
+      <c r="O40" s="13">
+        <f t="shared" si="4"/>
         <v>0.11747830023271844</v>
       </c>
-      <c r="P40" s="15">
-        <f>K6-N40</f>
+      <c r="P40" s="13">
+        <f t="shared" si="5"/>
         <v>0.18225661941967886</v>
       </c>
     </row>
@@ -5870,26 +5814,26 @@
       <c r="I41" s="2">
         <v>5</v>
       </c>
-      <c r="J41" s="16">
+      <c r="J41" s="14">
         <v>1001.2</v>
       </c>
       <c r="K41" s="2">
         <v>0.1</v>
       </c>
-      <c r="M41" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F7+1.5538</f>
+      <c r="M41" s="13">
+        <f t="shared" si="2"/>
         <v>4.0515281870636617</v>
       </c>
-      <c r="N41" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N7+0.5183</f>
+      <c r="N41" s="13">
+        <f t="shared" si="3"/>
         <v>7.16812952452874</v>
       </c>
-      <c r="O41" s="15">
-        <f>C7-M41</f>
+      <c r="O41" s="13">
+        <f t="shared" si="4"/>
         <v>-5.1128187063661734E-2</v>
       </c>
-      <c r="P41" s="15">
-        <f>K7-N41</f>
+      <c r="P41" s="13">
+        <f t="shared" si="5"/>
         <v>-0.16852952452873993</v>
       </c>
     </row>
@@ -5897,35 +5841,35 @@
       <c r="I42" s="2">
         <v>6</v>
       </c>
-      <c r="J42" s="16">
+      <c r="J42" s="14">
         <v>996.3</v>
       </c>
       <c r="K42" s="2">
         <v>0.1</v>
       </c>
-      <c r="M42" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F8+1.5538</f>
+      <c r="M42" s="13">
+        <f t="shared" si="2"/>
         <v>4.3845586120054882</v>
       </c>
-      <c r="N42" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N8+0.5183</f>
+      <c r="N42" s="13">
+        <f t="shared" si="3"/>
         <v>6.5193656684771577</v>
       </c>
-      <c r="O42" s="15">
-        <f>C8-M42</f>
+      <c r="O42" s="13">
+        <f t="shared" si="4"/>
         <v>0.61754138799451219</v>
       </c>
-      <c r="P42" s="15">
-        <f>K8-N42</f>
+      <c r="P42" s="13">
+        <f t="shared" si="5"/>
         <v>-0.5160656684771574</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B43" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="C43" s="29"/>
-      <c r="D43" s="21">
+      <c r="B43" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="19">
         <f>2*D38/I32</f>
         <v>67.909909909909913</v>
       </c>
@@ -5933,178 +5877,177 @@
       <c r="I43" s="2">
         <v>7</v>
       </c>
-      <c r="J43" s="16">
+      <c r="J43" s="14">
         <v>999.55</v>
       </c>
       <c r="K43" s="2">
         <v>0.1</v>
       </c>
-      <c r="M43" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F9+1.5538</f>
+      <c r="M43" s="13">
+        <f t="shared" si="2"/>
         <v>5.2171346743600422</v>
       </c>
-      <c r="N43" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N9+0.5183</f>
+      <c r="N43" s="13">
+        <f t="shared" si="3"/>
         <v>5.8706018124255657</v>
       </c>
-      <c r="O43" s="15">
-        <f>C9-M43</f>
+      <c r="O43" s="13">
+        <f t="shared" si="4"/>
         <v>0.78616532563995811</v>
       </c>
-      <c r="P43" s="15">
-        <f>K9-N43</f>
+      <c r="P43" s="13">
+        <f t="shared" si="5"/>
         <v>-0.86850181242556523</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.3">
       <c r="E44" s="4"/>
-      <c r="F44" s="30" t="s">
+      <c r="F44" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="G44" s="11" t="s">
+      <c r="G44" s="9" t="s">
         <v>4</v>
       </c>
       <c r="I44" s="2">
         <v>8</v>
       </c>
-      <c r="J44" s="16">
+      <c r="J44" s="14">
         <v>997.55</v>
       </c>
       <c r="K44" s="2">
         <v>0.1</v>
       </c>
-      <c r="M44" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F10+1.5538</f>
+      <c r="M44" s="13">
+        <f t="shared" si="2"/>
         <v>5.8831955242436829</v>
       </c>
-      <c r="N44" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N10+0.5183</f>
+      <c r="N44" s="13">
+        <f t="shared" si="3"/>
         <v>4.2486921722966047</v>
       </c>
-      <c r="O44" s="15">
-        <f>C10-M44</f>
+      <c r="O44" s="13">
+        <f t="shared" si="4"/>
         <v>1.1164044757563172</v>
       </c>
-      <c r="P44" s="15">
-        <f>K10-N44</f>
+      <c r="P44" s="13">
+        <f t="shared" si="5"/>
         <v>-0.24829217229660472</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D45" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="22"/>
-      <c r="F45" s="13">
-        <f>(SLOPE(C4:C13,F4:F13)*8*D38*H4*9.8)/(I32*PI()*D32^2)</f>
+      <c r="D45" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="23"/>
+      <c r="F45" s="11">
+        <f>(SLOPE(C4:C13,F4:F13)*8*D38*L32*9.8)/(I32*PI()*D32^2)</f>
         <v>135897756643.09407</v>
       </c>
-      <c r="G45" s="13">
-        <f>(SLOPE(K4:K13,N4:N13)*8*D38*H4*9.8)/(I32*PI()*D32^2)</f>
+      <c r="G45" s="11">
+        <f>(SLOPE(K4:K13,N4:N13)*8*D38*L32*9.8)/(I32*PI()*D32^2)</f>
         <v>132368615636.1472</v>
       </c>
       <c r="I45" s="2">
         <v>9</v>
       </c>
-      <c r="J45" s="16">
+      <c r="J45" s="14">
         <v>1000.7</v>
       </c>
       <c r="K45" s="2">
         <v>0.1</v>
       </c>
-      <c r="M45" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F11+1.5538</f>
+      <c r="M45" s="13">
+        <f t="shared" si="2"/>
         <v>8.3809237113073447</v>
       </c>
-      <c r="N45" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N11+0.5183</f>
+      <c r="N45" s="13">
+        <f t="shared" si="3"/>
         <v>2.7889734961805424</v>
       </c>
-      <c r="O45" s="15">
-        <f>C11-M45</f>
+      <c r="O45" s="13">
+        <f t="shared" si="4"/>
         <v>-0.3817737113073445</v>
       </c>
-      <c r="P45" s="15">
-        <f>K11-N45</f>
+      <c r="P45" s="13">
+        <f t="shared" si="5"/>
         <v>0.21442650381945771</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D46" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="E46" s="22"/>
-      <c r="F46" s="14">
+      <c r="D46" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" s="23"/>
+      <c r="F46" s="12">
         <f>ABS(F45-1.9*100000000000)/(1.9*100000000000)</f>
         <v>0.28474864924687332</v>
       </c>
-      <c r="G46" s="14">
+      <c r="G46" s="12">
         <f>ABS(G45-1.9*100000000000)/(1.9*100000000000)</f>
         <v>0.30332307559922528</v>
       </c>
       <c r="I46" s="2">
         <v>10</v>
       </c>
-      <c r="J46" s="16">
+      <c r="J46" s="14">
         <v>2003.35</v>
       </c>
       <c r="K46" s="2">
         <v>0.1</v>
       </c>
-      <c r="M46" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F12+1.5538</f>
+      <c r="M46" s="13">
+        <f t="shared" si="2"/>
         <v>9.0469845611909854</v>
       </c>
-      <c r="N46" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N12+0.5183</f>
+      <c r="N46" s="13">
+        <f t="shared" si="3"/>
         <v>1.8158277121031638</v>
       </c>
-      <c r="O46" s="15">
-        <f>C12-M46</f>
+      <c r="O46" s="13">
+        <f t="shared" si="4"/>
         <v>-5.0284561190984789E-2</v>
       </c>
-      <c r="P46" s="15">
-        <f>K12-N46</f>
+      <c r="P46" s="13">
+        <f t="shared" si="5"/>
         <v>0.18492228789683618</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="M47" s="15">
-        <f>SLOPE($C$4:$C$13,$F$4:$F$13)*F13+1.5538</f>
+      <c r="M47" s="13">
+        <f t="shared" si="2"/>
         <v>10.712136685900093</v>
       </c>
-      <c r="N47" s="15">
-        <f>SLOPE($K$4:$K$13,$N$4:$N$13)*N13+0.5183</f>
+      <c r="N47" s="13">
+        <f t="shared" si="3"/>
         <v>-0.29265482006448029</v>
       </c>
-      <c r="O47" s="15">
-        <f>C13-M47</f>
+      <c r="O47" s="13">
+        <f t="shared" si="4"/>
         <v>-0.71473668590009254</v>
       </c>
-      <c r="P47" s="15">
-        <f>K13-N47</f>
+      <c r="P47" s="13">
+        <f t="shared" si="5"/>
         <v>0.29265482006448029</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="16">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="J2:N2"/>
+    <mergeCell ref="D32:D35"/>
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="F32:F35"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="P3:Q9"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
     <mergeCell ref="M36:N36"/>
     <mergeCell ref="O36:P36"/>
     <mergeCell ref="B43:C43"/>
     <mergeCell ref="D45:E45"/>
     <mergeCell ref="D46:E46"/>
-    <mergeCell ref="P32:P34"/>
-    <mergeCell ref="P3:Q9"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="J2:N2"/>
-    <mergeCell ref="D32:D35"/>
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="F32:F35"/>
-    <mergeCell ref="N32:N34"/>
-    <mergeCell ref="O32:O34"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
T4B - Versão ainda mais final
</commit_message>
<xml_diff>
--- a/T4B - aço.xlsx
+++ b/T4B - aço.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nunop\OneDrive\Documentos\GitHub\LABSFISICAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B85112D-1167-4D91-A1FD-F77C2B0EC6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD1A6D5-FD5D-4A2B-B381-6519E0831E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB9F9942-6413-4E83-AC7B-C341FADCEB64}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Carga</t>
   </si>
@@ -150,6 +150,9 @@
   <si>
     <t>Coeficiente de Ampliação:</t>
   </si>
+  <si>
+    <t>Média</t>
+  </si>
 </sst>
 </file>
 
@@ -262,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,17 +325,20 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -340,15 +346,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5114,10 +5118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83617AA6-E6F3-42B7-BA6C-E56FF542CF9F}">
-  <dimension ref="B2:Q47"/>
+  <dimension ref="B2:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J48" sqref="J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5137,20 +5141,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="J2" s="27" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="J2" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
@@ -5183,10 +5187,10 @@
       <c r="N3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="P3" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="25"/>
+      <c r="Q3" s="26"/>
     </row>
     <row r="4" spans="2:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10">
@@ -5220,8 +5224,8 @@
         <f>($D$4-L4)*0.01</f>
         <v>5.5E-2</v>
       </c>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
+      <c r="P4" s="26"/>
+      <c r="Q4" s="26"/>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
@@ -5256,8 +5260,8 @@
         <f t="shared" ref="N5:N13" si="0">($D$4-L5)*0.01</f>
         <v>0.05</v>
       </c>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
     </row>
     <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -5293,8 +5297,8 @@
         <f t="shared" si="0"/>
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="P6" s="25"/>
-      <c r="Q6" s="25"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -5329,8 +5333,8 @@
         <f t="shared" si="0"/>
         <v>4.1000000000000016E-2</v>
       </c>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
     </row>
     <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -5365,8 +5369,8 @@
         <f t="shared" si="0"/>
         <v>3.7000000000000026E-2</v>
       </c>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
+      <c r="P8" s="26"/>
+      <c r="Q8" s="26"/>
     </row>
     <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -5401,8 +5405,8 @@
         <f t="shared" si="0"/>
         <v>3.2999999999999974E-2</v>
       </c>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="26"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -5568,10 +5572,10 @@
       <c r="J31" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L31" s="23" t="s">
+      <c r="L31" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="M31" s="23"/>
+      <c r="M31" s="21"/>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.3">
       <c r="B32" s="8">
@@ -5580,7 +5584,7 @@
       <c r="C32" s="8">
         <v>0.01</v>
       </c>
-      <c r="D32" s="28">
+      <c r="D32" s="23">
         <f>AVERAGE(B32:B36)*0.01</f>
         <v>8.7000000000000001E-4</v>
       </c>
@@ -5598,10 +5602,10 @@
       <c r="J32" s="18">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="L32" s="29">
+      <c r="L32" s="25">
         <v>0.72899999999999998</v>
       </c>
-      <c r="M32" s="29"/>
+      <c r="M32" s="25"/>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="8">
@@ -5610,7 +5614,7 @@
       <c r="C33" s="8">
         <v>0.01</v>
       </c>
-      <c r="D33" s="28"/>
+      <c r="D33" s="23"/>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
     </row>
@@ -5621,7 +5625,7 @@
       <c r="C34" s="8">
         <v>0.01</v>
       </c>
-      <c r="D34" s="28"/>
+      <c r="D34" s="23"/>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
     </row>
@@ -5632,7 +5636,7 @@
       <c r="C35" s="8">
         <v>0.01</v>
       </c>
-      <c r="D35" s="28"/>
+      <c r="D35" s="23"/>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
     </row>
@@ -5646,14 +5650,14 @@
       <c r="K36" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="M36" s="21" t="s">
+      <c r="M36" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="N36" s="22"/>
-      <c r="O36" s="21" t="s">
+      <c r="N36" s="29"/>
+      <c r="O36" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="P36" s="22"/>
+      <c r="P36" s="29"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="17" t="s">
@@ -5700,15 +5704,15 @@
       <c r="C38" s="8">
         <v>0.05</v>
       </c>
-      <c r="D38" s="26">
+      <c r="D38" s="27">
         <f>AVERAGE(B38:B40)*0.01</f>
         <v>2.5126666666666666</v>
       </c>
-      <c r="E38" s="26">
+      <c r="E38" s="27">
         <f>_xlfn.STDEV.P(B38:B40)</f>
         <v>0.69442222186665081</v>
       </c>
-      <c r="F38" s="26">
+      <c r="F38" s="27">
         <f>E38/SQRT(3)</f>
         <v>0.40092485672596889</v>
       </c>
@@ -5745,9 +5749,9 @@
       <c r="C39" s="8">
         <v>0.05</v>
       </c>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
       <c r="I39" s="2">
         <v>3</v>
       </c>
@@ -5781,9 +5785,9 @@
       <c r="C40" s="8">
         <v>0.05</v>
       </c>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="26"/>
+      <c r="D40" s="27"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="27"/>
       <c r="I40" s="2">
         <v>4</v>
       </c>
@@ -5865,10 +5869,10 @@
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="22"/>
+      <c r="C43" s="29"/>
       <c r="D43" s="19">
         <f>2*D38/I32</f>
         <v>67.909909909909913</v>
@@ -5901,13 +5905,6 @@
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="E44" s="4"/>
-      <c r="F44" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="G44" s="9" t="s">
-        <v>4</v>
-      </c>
       <c r="I44" s="2">
         <v>8</v>
       </c>
@@ -5935,18 +5932,6 @@
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D45" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E45" s="23"/>
-      <c r="F45" s="11">
-        <f>(SLOPE(C4:C13,F4:F13)*8*D38*L32*9.8)/(I32*PI()*D32^2)</f>
-        <v>135897756643.09407</v>
-      </c>
-      <c r="G45" s="11">
-        <f>(SLOPE(K4:K13,N4:N13)*8*D38*L32*9.8)/(I32*PI()*D32^2)</f>
-        <v>132368615636.1472</v>
-      </c>
       <c r="I45" s="2">
         <v>9</v>
       </c>
@@ -5974,18 +5959,6 @@
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="D46" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" s="23"/>
-      <c r="F46" s="12">
-        <f>ABS(F45-1.9*100000000000)/(1.9*100000000000)</f>
-        <v>0.28474864924687332</v>
-      </c>
-      <c r="G46" s="12">
-        <f>ABS(G45-1.9*100000000000)/(1.9*100000000000)</f>
-        <v>0.30332307559922528</v>
-      </c>
       <c r="I46" s="2">
         <v>10</v>
       </c>
@@ -6013,6 +5986,16 @@
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="D47" s="4"/>
+      <c r="E47" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="30" t="s">
+        <v>38</v>
+      </c>
       <c r="M47" s="13">
         <f t="shared" si="2"/>
         <v>10.712136685900093</v>
@@ -6030,8 +6013,53 @@
         <v>0.29265482006448029</v>
       </c>
     </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C48" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="11">
+        <f>(SLOPE(C4:C13,F4:F13)*8*D38*L32*9.8)/(I32*PI()*D32^2)</f>
+        <v>135897756643.09407</v>
+      </c>
+      <c r="F48" s="11">
+        <f>(SLOPE(K4:K13,N4:N13)*8*D38*L32*9.8)/(I32*PI()*D32^2)</f>
+        <v>132368615636.1472</v>
+      </c>
+      <c r="G48" s="19">
+        <f>AVERAGE(E48:F48)</f>
+        <v>134133186139.62064</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C49" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" s="21"/>
+      <c r="E49" s="12">
+        <f>ABS(E48-1.9*100000000000)/(1.9*100000000000)</f>
+        <v>0.28474864924687332</v>
+      </c>
+      <c r="F49" s="12">
+        <f>ABS(F48-1.9*100000000000)/(1.9*100000000000)</f>
+        <v>0.30332307559922528</v>
+      </c>
+      <c r="G49" s="12">
+        <f>ABS(G48-1.9*100000000000)/(1.9*100000000000)</f>
+        <v>0.2940358624230493</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="P3:Q9"/>
+    <mergeCell ref="D38:D40"/>
+    <mergeCell ref="E38:E40"/>
+    <mergeCell ref="F38:F40"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="O36:P36"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="J2:N2"/>
     <mergeCell ref="D32:D35"/>
@@ -6039,15 +6067,6 @@
     <mergeCell ref="F32:F35"/>
     <mergeCell ref="L31:M31"/>
     <mergeCell ref="L32:M32"/>
-    <mergeCell ref="P3:Q9"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="F38:F40"/>
-    <mergeCell ref="M36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>